<commit_message>
refactored stage data for canvas
</commit_message>
<xml_diff>
--- a/backend/emporium/data/StageData.xlsx
+++ b/backend/emporium/data/StageData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="828" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="828" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="income" sheetId="8" r:id="rId1"/>
@@ -60,9 +60,6 @@
     <t>World</t>
   </si>
   <si>
-    <t>Barrel</t>
-  </si>
-  <si>
     <t>Mig</t>
   </si>
   <si>
@@ -73,9 +70,6 @@
   </si>
   <si>
     <t>Gargoyle</t>
-  </si>
-  <si>
-    <t>Window</t>
   </si>
   <si>
     <t>Idol</t>
@@ -97,9 +91,6 @@
   </si>
   <si>
     <t>Spike Trap</t>
-  </si>
-  <si>
-    <t>Chandelier</t>
   </si>
   <si>
     <t>Chest</t>
@@ -268,6 +259,15 @@
   </si>
   <si>
     <t>world</t>
+  </si>
+  <si>
+    <t>Balcony</t>
+  </si>
+  <si>
+    <t>Rat Swarm</t>
+  </si>
+  <si>
+    <t>Sewer Grate</t>
   </si>
 </sst>
 </file>
@@ -642,7 +642,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -653,22 +653,22 @@
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -869,7 +869,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I79"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J1" sqref="J1"/>
     </sheetView>
@@ -886,7 +886,7 @@
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -918,19 +918,19 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G3" s="1">
         <v>8</v>
@@ -947,19 +947,19 @@
         <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="D4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>14</v>
-      </c>
       <c r="F4" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G4" s="1">
         <v>8</v>
@@ -976,19 +976,19 @@
         <v>1</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>24</v>
+        <v>78</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>21</v>
-      </c>
       <c r="F5" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G5" s="1">
         <v>8</v>
@@ -1005,19 +1005,19 @@
         <v>1</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G6" s="1">
         <v>8</v>
@@ -1034,19 +1034,19 @@
         <v>1</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G7" s="1">
         <v>8</v>
@@ -1063,19 +1063,19 @@
         <v>1</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="D8" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G8" s="1">
         <v>8</v>
@@ -1092,19 +1092,19 @@
         <v>1</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="5" t="s">
-        <v>21</v>
-      </c>
       <c r="F9" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G9" s="1">
         <v>8</v>
@@ -1121,19 +1121,19 @@
         <v>1</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G10" s="1">
         <v>8</v>
@@ -1150,19 +1150,19 @@
         <v>1</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>14</v>
-      </c>
       <c r="F11" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G11" s="1">
         <v>8</v>
@@ -1179,19 +1179,19 @@
         <v>1</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G12" s="1">
         <v>8</v>
@@ -1208,19 +1208,19 @@
         <v>1</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="E13" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G13" s="1">
         <v>8</v>
@@ -1237,19 +1237,19 @@
         <v>1</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="E14" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G14" s="1">
         <v>8</v>
@@ -1266,19 +1266,19 @@
         <v>2</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G16" s="1">
         <v>8</v>
@@ -1295,19 +1295,19 @@
         <v>2</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="D17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E17" s="5" t="s">
-        <v>14</v>
-      </c>
       <c r="F17" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G17" s="1">
         <v>8</v>
@@ -1324,19 +1324,19 @@
         <v>2</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>24</v>
+        <v>78</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E18" s="5" t="s">
-        <v>21</v>
-      </c>
       <c r="F18" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G18" s="1">
         <v>8</v>
@@ -1353,19 +1353,19 @@
         <v>2</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G19" s="1">
         <v>8</v>
@@ -1382,19 +1382,19 @@
         <v>2</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G20" s="1">
         <v>8</v>
@@ -1411,19 +1411,19 @@
         <v>2</v>
       </c>
       <c r="B21" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="D21" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G21" s="1">
         <v>8</v>
@@ -1440,19 +1440,19 @@
         <v>2</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E22" s="5" t="s">
-        <v>21</v>
-      </c>
       <c r="F22" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G22" s="1">
         <v>8</v>
@@ -1469,19 +1469,19 @@
         <v>2</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G23" s="1">
         <v>8</v>
@@ -1498,19 +1498,19 @@
         <v>2</v>
       </c>
       <c r="B24" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="D24" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="E24" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E24" s="5" t="s">
-        <v>14</v>
-      </c>
       <c r="F24" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G24" s="1">
         <v>8</v>
@@ -1527,19 +1527,19 @@
         <v>2</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G25" s="1">
         <v>8</v>
@@ -1556,19 +1556,19 @@
         <v>2</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="E26" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G26" s="1">
         <v>8</v>
@@ -1585,19 +1585,19 @@
         <v>2</v>
       </c>
       <c r="B27" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="E27" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G27" s="1">
         <v>8</v>
@@ -1614,19 +1614,19 @@
         <v>4</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G29" s="1">
         <v>9</v>
@@ -1643,19 +1643,19 @@
         <v>4</v>
       </c>
       <c r="B30" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="D30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E30" s="5" t="s">
-        <v>14</v>
-      </c>
       <c r="F30" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G30" s="1">
         <v>9</v>
@@ -1672,19 +1672,19 @@
         <v>4</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>24</v>
+        <v>78</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D31" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E31" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E31" s="5" t="s">
-        <v>21</v>
-      </c>
       <c r="F31" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G31" s="1">
         <v>9</v>
@@ -1701,19 +1701,19 @@
         <v>4</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G32" s="1">
         <v>9</v>
@@ -1730,19 +1730,19 @@
         <v>4</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G33" s="1">
         <v>9</v>
@@ -1759,19 +1759,19 @@
         <v>4</v>
       </c>
       <c r="B34" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="D34" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G34" s="1">
         <v>9</v>
@@ -1788,19 +1788,19 @@
         <v>4</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D35" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E35" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E35" s="5" t="s">
-        <v>21</v>
-      </c>
       <c r="F35" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G35" s="1">
         <v>9</v>
@@ -1817,19 +1817,19 @@
         <v>4</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G36" s="1">
         <v>9</v>
@@ -1846,19 +1846,19 @@
         <v>4</v>
       </c>
       <c r="B37" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="D37" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="E37" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E37" s="5" t="s">
-        <v>14</v>
-      </c>
       <c r="F37" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G37" s="1">
         <v>9</v>
@@ -1875,19 +1875,19 @@
         <v>4</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G38" s="1">
         <v>9</v>
@@ -1904,19 +1904,19 @@
         <v>4</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="C39" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D39" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="E39" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G39" s="1">
         <v>9</v>
@@ -1933,19 +1933,19 @@
         <v>4</v>
       </c>
       <c r="B40" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="E40" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G40" s="1">
         <v>9</v>
@@ -1962,19 +1962,19 @@
         <v>5</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G42" s="1">
         <v>9</v>
@@ -1991,19 +1991,19 @@
         <v>5</v>
       </c>
       <c r="B43" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C43" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="D43" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E43" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E43" s="5" t="s">
-        <v>14</v>
-      </c>
       <c r="F43" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G43" s="1">
         <v>9</v>
@@ -2020,19 +2020,19 @@
         <v>5</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>24</v>
+        <v>78</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D44" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E44" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E44" s="5" t="s">
-        <v>21</v>
-      </c>
       <c r="F44" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G44" s="1">
         <v>9</v>
@@ -2049,19 +2049,19 @@
         <v>5</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G45" s="1">
         <v>9</v>
@@ -2078,19 +2078,19 @@
         <v>5</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G46" s="1">
         <v>9</v>
@@ -2107,19 +2107,19 @@
         <v>5</v>
       </c>
       <c r="B47" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C47" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="D47" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G47" s="1">
         <v>9</v>
@@ -2136,19 +2136,19 @@
         <v>5</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D48" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E48" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E48" s="5" t="s">
-        <v>21</v>
-      </c>
       <c r="F48" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G48" s="1">
         <v>9</v>
@@ -2165,19 +2165,19 @@
         <v>5</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G49" s="1">
         <v>9</v>
@@ -2194,19 +2194,19 @@
         <v>5</v>
       </c>
       <c r="B50" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C50" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="D50" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="E50" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E50" s="5" t="s">
-        <v>14</v>
-      </c>
       <c r="F50" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G50" s="1">
         <v>9</v>
@@ -2223,19 +2223,19 @@
         <v>5</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G51" s="1">
         <v>9</v>
@@ -2252,19 +2252,19 @@
         <v>5</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="C52" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D52" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D52" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="E52" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G52" s="1">
         <v>9</v>
@@ -2281,19 +2281,19 @@
         <v>5</v>
       </c>
       <c r="B53" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C53" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="E53" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G53" s="1">
         <v>9</v>
@@ -2310,19 +2310,19 @@
         <v>7</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G55" s="1">
         <v>10</v>
@@ -2339,19 +2339,19 @@
         <v>7</v>
       </c>
       <c r="B56" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C56" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="D56" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E56" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E56" s="5" t="s">
-        <v>14</v>
-      </c>
       <c r="F56" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G56" s="1">
         <v>10</v>
@@ -2368,19 +2368,19 @@
         <v>7</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>24</v>
+        <v>78</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D57" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E57" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E57" s="5" t="s">
-        <v>21</v>
-      </c>
       <c r="F57" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G57" s="1">
         <v>10</v>
@@ -2397,19 +2397,19 @@
         <v>7</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G58" s="1">
         <v>10</v>
@@ -2426,19 +2426,19 @@
         <v>7</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G59" s="1">
         <v>10</v>
@@ -2455,19 +2455,19 @@
         <v>7</v>
       </c>
       <c r="B60" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C60" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C60" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="D60" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G60" s="1">
         <v>10</v>
@@ -2484,19 +2484,19 @@
         <v>7</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D61" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E61" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E61" s="5" t="s">
-        <v>21</v>
-      </c>
       <c r="F61" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G61" s="1">
         <v>10</v>
@@ -2513,19 +2513,19 @@
         <v>7</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G62" s="1">
         <v>10</v>
@@ -2542,19 +2542,19 @@
         <v>7</v>
       </c>
       <c r="B63" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C63" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="D63" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D63" s="1" t="s">
+      <c r="E63" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E63" s="5" t="s">
-        <v>14</v>
-      </c>
       <c r="F63" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G63" s="1">
         <v>10</v>
@@ -2571,19 +2571,19 @@
         <v>7</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G64" s="1">
         <v>10</v>
@@ -2600,19 +2600,19 @@
         <v>7</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="C65" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D65" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D65" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="E65" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G65" s="1">
         <v>10</v>
@@ -2629,19 +2629,19 @@
         <v>7</v>
       </c>
       <c r="B66" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D66" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C66" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="E66" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G66" s="1">
         <v>10</v>
@@ -2658,19 +2658,19 @@
         <v>8</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F68" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G68" s="1">
         <v>10</v>
@@ -2687,19 +2687,19 @@
         <v>8</v>
       </c>
       <c r="B69" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C69" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C69" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="D69" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E69" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E69" s="5" t="s">
-        <v>14</v>
-      </c>
       <c r="F69" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G69" s="1">
         <v>10</v>
@@ -2716,19 +2716,19 @@
         <v>8</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>24</v>
+        <v>78</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D70" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E70" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E70" s="5" t="s">
-        <v>21</v>
-      </c>
       <c r="F70" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G70" s="1">
         <v>10</v>
@@ -2745,19 +2745,19 @@
         <v>8</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E71" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G71" s="1">
         <v>10</v>
@@ -2774,19 +2774,19 @@
         <v>8</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E72" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F72" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G72" s="1">
         <v>10</v>
@@ -2803,19 +2803,19 @@
         <v>8</v>
       </c>
       <c r="B73" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C73" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C73" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="D73" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G73" s="1">
         <v>10</v>
@@ -2832,19 +2832,19 @@
         <v>8</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D74" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E74" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E74" s="5" t="s">
-        <v>21</v>
-      </c>
       <c r="F74" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G74" s="1">
         <v>10</v>
@@ -2861,19 +2861,19 @@
         <v>8</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F75" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G75" s="1">
         <v>10</v>
@@ -2890,19 +2890,19 @@
         <v>8</v>
       </c>
       <c r="B76" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C76" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C76" s="1" t="s">
+      <c r="D76" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D76" s="1" t="s">
+      <c r="E76" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E76" s="5" t="s">
-        <v>14</v>
-      </c>
       <c r="F76" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G76" s="1">
         <v>10</v>
@@ -2919,19 +2919,19 @@
         <v>8</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E77" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F77" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G77" s="1">
         <v>10</v>
@@ -2948,19 +2948,19 @@
         <v>8</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="C78" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D78" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D78" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="E78" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G78" s="1">
         <v>10</v>
@@ -2977,19 +2977,19 @@
         <v>8</v>
       </c>
       <c r="B79" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D79" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C79" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="E79" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F79" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G79" s="1">
         <v>10</v>
@@ -3029,7 +3029,7 @@
   <sheetData>
     <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -3059,10 +3059,10 @@
         <v>3</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
@@ -3070,19 +3070,19 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G3" s="1">
         <f>ROUND(8* 1.6,0)</f>
@@ -3110,19 +3110,19 @@
         <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G4" s="1">
         <f t="shared" ref="G4:G5" si="0">ROUND(8* 1.6,0)</f>
@@ -3150,19 +3150,19 @@
         <v>1</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G5" s="1">
         <f t="shared" si="0"/>
@@ -3193,19 +3193,19 @@
         <v>2</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G7" s="1">
         <f>ROUND(8* 1.6,0)</f>
@@ -3233,19 +3233,19 @@
         <v>2</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G8" s="1">
         <f t="shared" ref="G8:G9" si="2">ROUND(8* 1.6,0)</f>
@@ -3273,19 +3273,19 @@
         <v>2</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G9" s="1">
         <f t="shared" si="2"/>
@@ -3313,19 +3313,19 @@
         <v>4</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G11" s="1">
         <f>ROUND(9* 1.6,0)</f>
@@ -3353,19 +3353,19 @@
         <v>4</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G12" s="1">
         <f t="shared" ref="G12:G13" si="3">ROUND(9* 1.6,0)</f>
@@ -3393,19 +3393,19 @@
         <v>4</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G13" s="1">
         <f t="shared" si="3"/>
@@ -3433,19 +3433,19 @@
         <v>5</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G15" s="1">
         <f>ROUND(9* 1.6,0)</f>
@@ -3473,19 +3473,19 @@
         <v>5</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G16" s="1">
         <f t="shared" ref="G16:G17" si="4">ROUND(9* 1.6,0)</f>
@@ -3513,19 +3513,19 @@
         <v>5</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G17" s="1">
         <f t="shared" si="4"/>
@@ -3553,19 +3553,19 @@
         <v>7</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G19" s="1">
         <f>ROUND(10* 1.6,0)</f>
@@ -3593,19 +3593,19 @@
         <v>7</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G20" s="1">
         <f>ROUND(10* 1.6,0)</f>
@@ -3633,19 +3633,19 @@
         <v>7</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G21" s="1">
         <f>ROUND(10* 1.6,0)</f>
@@ -3673,19 +3673,19 @@
         <v>8</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G23" s="1">
         <f>ROUND(10* 1.6,0)</f>
@@ -3713,19 +3713,19 @@
         <v>8</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G24" s="1">
         <f>ROUND(10* 1.6,0)</f>
@@ -3753,19 +3753,19 @@
         <v>8</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G25" s="1">
         <f>ROUND(10* 1.6,0)</f>
@@ -3813,58 +3813,58 @@
   <sheetData>
     <row r="1" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="P1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="N1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
@@ -5661,58 +5661,58 @@
   <sheetData>
     <row r="1" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="P1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="N1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
@@ -6778,55 +6778,55 @@
         <v>10</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="P1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="N1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
@@ -8627,7 +8627,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -8639,66 +8639,66 @@
   <sheetData>
     <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
market page inventory backend created
</commit_message>
<xml_diff>
--- a/backend/emporium/data/StageData.xlsx
+++ b/backend/emporium/data/StageData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="828" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="828" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="income" sheetId="8" r:id="rId1"/>
@@ -4462,7 +4462,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="S1" sqref="S1"/>
     </sheetView>
@@ -7334,9 +7334,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S1" sqref="S1"/>
+      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
cloaks added to items
</commit_message>
<xml_diff>
--- a/backend/emporium/data/StageData.xlsx
+++ b/backend/emporium/data/StageData.xlsx
@@ -744,7 +744,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -761,16 +761,16 @@
         <v>53</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -785,180 +785,45 @@
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="1">
-        <v>110</v>
-      </c>
-      <c r="C3" s="1">
-        <v>4</v>
-      </c>
-      <c r="D3" s="1">
-        <v>35</v>
-      </c>
-      <c r="E3" s="1">
-        <v>14</v>
-      </c>
-      <c r="F3" s="1">
-        <v>7</v>
-      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
-      </c>
-      <c r="B4" s="1">
-        <v>124</v>
-      </c>
-      <c r="C4" s="1">
-        <v>4</v>
-      </c>
-      <c r="D4" s="1">
-        <v>37</v>
-      </c>
-      <c r="E4" s="1">
-        <v>16</v>
-      </c>
-      <c r="F4" s="1">
-        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="1">
-        <v>138</v>
-      </c>
-      <c r="C5" s="1">
-        <v>5</v>
-      </c>
-      <c r="D5" s="1">
-        <v>39</v>
-      </c>
-      <c r="E5" s="1">
-        <v>18</v>
-      </c>
-      <c r="F5" s="1">
-        <v>9</v>
-      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="1">
-        <v>152</v>
-      </c>
-      <c r="C6" s="1">
-        <v>5</v>
-      </c>
-      <c r="D6" s="1">
-        <v>41</v>
-      </c>
-      <c r="E6" s="1">
-        <v>20</v>
-      </c>
-      <c r="F6" s="1">
-        <v>10</v>
-      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="1">
-        <v>166</v>
-      </c>
-      <c r="C7" s="1">
-        <v>6</v>
-      </c>
-      <c r="D7" s="1">
-        <v>43</v>
-      </c>
-      <c r="E7" s="1">
-        <v>22</v>
-      </c>
-      <c r="F7" s="1">
-        <v>11</v>
-      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="1">
-        <v>180</v>
-      </c>
-      <c r="C8" s="1">
-        <v>6</v>
-      </c>
-      <c r="D8" s="1">
-        <v>45</v>
-      </c>
-      <c r="E8" s="1">
-        <v>24</v>
-      </c>
-      <c r="F8" s="1">
-        <v>12</v>
-      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" s="1">
-        <v>194</v>
-      </c>
-      <c r="C9" s="1">
-        <v>7</v>
-      </c>
-      <c r="D9" s="1">
-        <v>47</v>
-      </c>
-      <c r="E9" s="1">
-        <v>26</v>
-      </c>
-      <c r="F9" s="1">
-        <v>13</v>
-      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>8</v>
-      </c>
-      <c r="B10" s="1">
-        <v>208</v>
-      </c>
-      <c r="C10" s="1">
-        <v>7</v>
-      </c>
-      <c r="D10" s="1">
-        <v>49</v>
-      </c>
-      <c r="E10" s="1">
-        <v>28</v>
-      </c>
-      <c r="F10" s="1">
-        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>9</v>
-      </c>
-      <c r="B11" s="1">
-        <v>222</v>
-      </c>
-      <c r="C11" s="1">
-        <v>8</v>
-      </c>
-      <c r="D11" s="1">
-        <v>51</v>
-      </c>
-      <c r="E11" s="1">
-        <v>30</v>
-      </c>
-      <c r="F11" s="1">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -4557,15 +4422,15 @@
       </c>
       <c r="N3" s="7">
         <f>ROUND(income!$B$3 * $M3, 0)</f>
-        <v>110</v>
+        <v>0</v>
       </c>
       <c r="O3" s="7">
+        <f>ROUND(income!$F$3 * $M3, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P3" s="7">
         <f>ROUND(income!$C$3 * $M3, 0)</f>
-        <v>4</v>
-      </c>
-      <c r="P3" s="7">
-        <f>ROUND(income!$D$3 * $M3, 0)</f>
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="Q3" s="7">
         <v>0</v>
@@ -4603,15 +4468,15 @@
       </c>
       <c r="N4" s="7">
         <f>ROUND(income!$B$3 * M4, 0)</f>
-        <v>116</v>
+        <v>0</v>
       </c>
       <c r="O4" s="7">
+        <f>ROUND(income!$F$3 * $M4, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P4" s="7">
         <f>ROUND(income!$C$3 * $M4, 0)</f>
-        <v>4</v>
-      </c>
-      <c r="P4" s="7">
-        <f>ROUND(income!$D$3 * $M4, 0)</f>
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="Q4" s="7">
         <v>0</v>
@@ -4649,15 +4514,15 @@
       </c>
       <c r="N5" s="7">
         <f>ROUND(income!$B$3 * M5, 0)</f>
-        <v>121</v>
+        <v>0</v>
       </c>
       <c r="O5" s="7">
+        <f>ROUND(income!$F$3 * $M5, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P5" s="7">
         <f>ROUND(income!$C$3 * $M5, 0)</f>
-        <v>4</v>
-      </c>
-      <c r="P5" s="7">
-        <f>ROUND(income!$D$3 * $M5, 0)</f>
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="Q5" s="7">
         <v>0</v>
@@ -4695,15 +4560,15 @@
       </c>
       <c r="N6" s="7">
         <f>ROUND(income!$B$3 * M6, 0)</f>
-        <v>127</v>
+        <v>0</v>
       </c>
       <c r="O6" s="7">
+        <f>ROUND(income!$F$3 * $M6, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P6" s="7">
         <f>ROUND(income!$C$3 * $M6, 0)</f>
-        <v>5</v>
-      </c>
-      <c r="P6" s="7">
-        <f>ROUND(income!$D$3 * $M6, 0)</f>
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="Q6" s="7">
         <v>0</v>
@@ -4741,15 +4606,15 @@
       </c>
       <c r="N7" s="7">
         <f>ROUND(income!$B$3 * M7, 0)</f>
-        <v>132</v>
+        <v>0</v>
       </c>
       <c r="O7" s="7">
+        <f>ROUND(income!$F$3 * $M7, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P7" s="7">
         <f>ROUND(income!$C$3 * $M7, 0)</f>
-        <v>5</v>
-      </c>
-      <c r="P7" s="7">
-        <f>ROUND(income!$D$3 * $M7, 0)</f>
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="Q7" s="7">
         <v>0</v>
@@ -4790,15 +4655,15 @@
       </c>
       <c r="N8" s="7">
         <f>ROUND(income!$B$3 * M8, 0)</f>
-        <v>198</v>
+        <v>0</v>
       </c>
       <c r="O8" s="7">
+        <f>ROUND(income!$F$3 * $M8, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P8" s="7">
         <f>ROUND(income!$C$3 * $M8, 0)</f>
-        <v>7</v>
-      </c>
-      <c r="P8" s="7">
-        <f>ROUND(income!$D$3 * $M8, 0)</f>
-        <v>63</v>
+        <v>0</v>
       </c>
       <c r="Q8" s="7">
         <v>0</v>
@@ -4840,15 +4705,15 @@
       </c>
       <c r="N9" s="7">
         <f>ROUND(income!$B$3 * M9, 0)</f>
-        <v>209</v>
+        <v>0</v>
       </c>
       <c r="O9" s="7">
+        <f>ROUND(income!$F$3 * $M9, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P9" s="7">
         <f>ROUND(income!$C$3 * $M9, 0)</f>
-        <v>8</v>
-      </c>
-      <c r="P9" s="7">
-        <f>ROUND(income!$D$3 * $M9, 0)</f>
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="Q9" s="7">
         <v>0</v>
@@ -4890,15 +4755,15 @@
       </c>
       <c r="N10" s="7">
         <f>ROUND(income!$B$3 * M10, 0)</f>
-        <v>220</v>
+        <v>0</v>
       </c>
       <c r="O10" s="7">
+        <f>ROUND(income!$F$3 * $M10, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P10" s="7">
         <f>ROUND(income!$C$3 * $M10, 0)</f>
-        <v>8</v>
-      </c>
-      <c r="P10" s="7">
-        <f>ROUND(income!$D$3 * $M10, 0)</f>
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="Q10" s="7">
         <v>0</v>
@@ -4940,15 +4805,15 @@
       </c>
       <c r="N11" s="7">
         <f>ROUND(income!$B$3 * M11, 0)</f>
-        <v>231</v>
+        <v>0</v>
       </c>
       <c r="O11" s="7">
+        <f>ROUND(income!$F$3 * $M11, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P11" s="7">
         <f>ROUND(income!$C$3 * $M11, 0)</f>
-        <v>8</v>
-      </c>
-      <c r="P11" s="7">
-        <f>ROUND(income!$D$3 * $M11, 0)</f>
-        <v>74</v>
+        <v>0</v>
       </c>
       <c r="Q11" s="7">
         <v>0</v>
@@ -4989,19 +4854,19 @@
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
       <c r="M12" s="8">
-        <v>2.6</v>
+        <v>2.8</v>
       </c>
       <c r="N12" s="7">
         <f>ROUND(income!$B$3 * M12, 0)</f>
-        <v>286</v>
+        <v>0</v>
       </c>
       <c r="O12" s="7">
+        <f>ROUND(income!$F$3 * $M12, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P12" s="7">
         <f>ROUND(income!$C$3 * $M12, 0)</f>
-        <v>10</v>
-      </c>
-      <c r="P12" s="7">
-        <f>ROUND(income!$D$3 * $M12, 0)</f>
-        <v>91</v>
+        <v>0</v>
       </c>
       <c r="Q12" s="7">
         <v>0</v>
@@ -5042,20 +4907,19 @@
       <c r="K13" s="7"/>
       <c r="L13" s="7"/>
       <c r="M13" s="8">
-        <f>M12+0.2</f>
-        <v>2.8000000000000003</v>
+        <v>3</v>
       </c>
       <c r="N13" s="7">
         <f>ROUND(income!$B$3 * M13, 0)</f>
-        <v>308</v>
+        <v>0</v>
       </c>
       <c r="O13" s="7">
+        <f>ROUND(income!$F$3 * $M13, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P13" s="7">
         <f>ROUND(income!$C$3 * $M13, 0)</f>
-        <v>11</v>
-      </c>
-      <c r="P13" s="7">
-        <f>ROUND(income!$D$3 * $M13, 0)</f>
-        <v>98</v>
+        <v>0</v>
       </c>
       <c r="Q13" s="7">
         <v>0</v>
@@ -5097,19 +4961,19 @@
       <c r="L14" s="7"/>
       <c r="M14" s="8">
         <f>M13+0.2</f>
-        <v>3.0000000000000004</v>
+        <v>3.2</v>
       </c>
       <c r="N14" s="7">
         <f>ROUND(income!$B$3 * M14, 0)</f>
-        <v>330</v>
+        <v>0</v>
       </c>
       <c r="O14" s="7">
+        <f>ROUND(income!$F$3 * $M14, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P14" s="7">
         <f>ROUND(income!$C$3 * $M14, 0)</f>
-        <v>12</v>
-      </c>
-      <c r="P14" s="7">
-        <f>ROUND(income!$D$3 * $M14, 0)</f>
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="Q14" s="7">
         <v>0</v>
@@ -5148,15 +5012,15 @@
       </c>
       <c r="N16" s="7">
         <f>ROUND(income!$B$4 * $M16, 0)</f>
-        <v>124</v>
+        <v>0</v>
       </c>
       <c r="O16" s="7">
+        <f>ROUND(income!$F$4 * $M16, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P16" s="7">
         <f>ROUND(income!$C$4 * $M16, 0)</f>
-        <v>4</v>
-      </c>
-      <c r="P16" s="7">
-        <f>ROUND(income!$D$4 * $M16, 0)</f>
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="Q16" s="7">
         <v>0</v>
@@ -5194,15 +5058,15 @@
       </c>
       <c r="N17" s="7">
         <f>ROUND(income!$B$4 * $M17, 0)</f>
-        <v>130</v>
+        <v>0</v>
       </c>
       <c r="O17" s="7">
+        <f>ROUND(income!$F$4 * $M17, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P17" s="7">
         <f>ROUND(income!$C$4 * $M17, 0)</f>
-        <v>4</v>
-      </c>
-      <c r="P17" s="7">
-        <f>ROUND(income!$D$4 * $M17, 0)</f>
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="Q17" s="7">
         <v>0</v>
@@ -5240,15 +5104,15 @@
       </c>
       <c r="N18" s="7">
         <f>ROUND(income!$B$4 * $M18, 0)</f>
-        <v>136</v>
+        <v>0</v>
       </c>
       <c r="O18" s="7">
+        <f>ROUND(income!$F$4 * $M18, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P18" s="7">
         <f>ROUND(income!$C$4 * $M18, 0)</f>
-        <v>4</v>
-      </c>
-      <c r="P18" s="7">
-        <f>ROUND(income!$D$4 * $M18, 0)</f>
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="Q18" s="7">
         <v>0</v>
@@ -5286,15 +5150,15 @@
       </c>
       <c r="N19" s="7">
         <f>ROUND(income!$B$4 * $M19, 0)</f>
-        <v>143</v>
+        <v>0</v>
       </c>
       <c r="O19" s="7">
+        <f>ROUND(income!$F$4 * $M19, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P19" s="7">
         <f>ROUND(income!$C$4 * $M19, 0)</f>
-        <v>5</v>
-      </c>
-      <c r="P19" s="7">
-        <f>ROUND(income!$D$4 * $M19, 0)</f>
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="Q19" s="7">
         <v>0</v>
@@ -5332,15 +5196,15 @@
       </c>
       <c r="N20" s="7">
         <f>ROUND(income!$B$4 * $M20, 0)</f>
-        <v>149</v>
+        <v>0</v>
       </c>
       <c r="O20" s="7">
+        <f>ROUND(income!$F$4 * $M20, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P20" s="7">
         <f>ROUND(income!$C$4 * $M20, 0)</f>
-        <v>5</v>
-      </c>
-      <c r="P20" s="7">
-        <f>ROUND(income!$D$4 * $M20, 0)</f>
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="Q20" s="7">
         <v>0</v>
@@ -5381,15 +5245,15 @@
       </c>
       <c r="N21" s="7">
         <f>ROUND(income!$B$4 * $M21, 0)</f>
-        <v>223</v>
+        <v>0</v>
       </c>
       <c r="O21" s="7">
+        <f>ROUND(income!$F$4 * $M21, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P21" s="7">
         <f>ROUND(income!$C$4 * $M21, 0)</f>
-        <v>7</v>
-      </c>
-      <c r="P21" s="7">
-        <f>ROUND(income!$D$4 * $M21, 0)</f>
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="Q21" s="7">
         <v>0</v>
@@ -5431,15 +5295,15 @@
       </c>
       <c r="N22" s="7">
         <f>ROUND(income!$B$4 * $M22, 0)</f>
-        <v>236</v>
+        <v>0</v>
       </c>
       <c r="O22" s="7">
+        <f>ROUND(income!$F$4 * $M22, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P22" s="7">
         <f>ROUND(income!$C$4 * $M22, 0)</f>
-        <v>8</v>
-      </c>
-      <c r="P22" s="7">
-        <f>ROUND(income!$D$4 * $M22, 0)</f>
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="Q22" s="7">
         <v>0</v>
@@ -5481,15 +5345,15 @@
       </c>
       <c r="N23" s="7">
         <f>ROUND(income!$B$4 * $M23, 0)</f>
-        <v>248</v>
+        <v>0</v>
       </c>
       <c r="O23" s="7">
+        <f>ROUND(income!$F$4 * $M23, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P23" s="7">
         <f>ROUND(income!$C$4 * $M23, 0)</f>
-        <v>8</v>
-      </c>
-      <c r="P23" s="7">
-        <f>ROUND(income!$D$4 * $M23, 0)</f>
-        <v>74</v>
+        <v>0</v>
       </c>
       <c r="Q23" s="7">
         <v>0</v>
@@ -5531,15 +5395,15 @@
       </c>
       <c r="N24" s="7">
         <f>ROUND(income!$B$4 * $M24, 0)</f>
-        <v>260</v>
+        <v>0</v>
       </c>
       <c r="O24" s="7">
+        <f>ROUND(income!$F$4 * $M24, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P24" s="7">
         <f>ROUND(income!$C$4 * $M24, 0)</f>
-        <v>8</v>
-      </c>
-      <c r="P24" s="7">
-        <f>ROUND(income!$D$4 * $M24, 0)</f>
-        <v>78</v>
+        <v>0</v>
       </c>
       <c r="Q24" s="7">
         <v>0</v>
@@ -5580,19 +5444,19 @@
       <c r="K25" s="7"/>
       <c r="L25" s="7"/>
       <c r="M25" s="8">
-        <v>2.6</v>
+        <v>2.8</v>
       </c>
       <c r="N25" s="7">
         <f>ROUND(income!$B$4 * $M25, 0)</f>
-        <v>322</v>
+        <v>0</v>
       </c>
       <c r="O25" s="7">
+        <f>ROUND(income!$F$4 * $M25, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P25" s="7">
         <f>ROUND(income!$C$4 * $M25, 0)</f>
-        <v>10</v>
-      </c>
-      <c r="P25" s="7">
-        <f>ROUND(income!$D$4 * $M25, 0)</f>
-        <v>96</v>
+        <v>0</v>
       </c>
       <c r="Q25" s="7">
         <v>0</v>
@@ -5633,20 +5497,19 @@
       <c r="K26" s="7"/>
       <c r="L26" s="7"/>
       <c r="M26" s="8">
-        <f>M25+0.2</f>
-        <v>2.8000000000000003</v>
+        <v>3</v>
       </c>
       <c r="N26" s="7">
         <f>ROUND(income!$B$4 * $M26, 0)</f>
-        <v>347</v>
+        <v>0</v>
       </c>
       <c r="O26" s="7">
+        <f>ROUND(income!$F$4 * $M26, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P26" s="7">
         <f>ROUND(income!$C$4 * $M26, 0)</f>
-        <v>11</v>
-      </c>
-      <c r="P26" s="7">
-        <f>ROUND(income!$D$4 * $M26, 0)</f>
-        <v>104</v>
+        <v>0</v>
       </c>
       <c r="Q26" s="7">
         <v>0</v>
@@ -5688,19 +5551,19 @@
       <c r="L27" s="7"/>
       <c r="M27" s="8">
         <f>M26+0.2</f>
-        <v>3.0000000000000004</v>
+        <v>3.2</v>
       </c>
       <c r="N27" s="7">
         <f>ROUND(income!$B$4 * $M27, 0)</f>
-        <v>372</v>
+        <v>0</v>
       </c>
       <c r="O27" s="7">
+        <f>ROUND(income!$F$4 * $M27, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P27" s="7">
         <f>ROUND(income!$C$4 * $M27, 0)</f>
-        <v>12</v>
-      </c>
-      <c r="P27" s="7">
-        <f>ROUND(income!$D$4 * $M27, 0)</f>
-        <v>111</v>
+        <v>0</v>
       </c>
       <c r="Q27" s="7">
         <v>0</v>
@@ -5739,15 +5602,15 @@
       </c>
       <c r="N29" s="7">
         <f>ROUND(income!$B$5 * $M29, 0)</f>
-        <v>138</v>
+        <v>0</v>
       </c>
       <c r="O29" s="7">
+        <f>ROUND(income!$F$5 * $M29, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P29" s="7">
         <f>ROUND(income!$C$5 * $M29, 0)</f>
-        <v>5</v>
-      </c>
-      <c r="P29" s="7">
-        <f>ROUND(income!$D$5 * $M29, 0)</f>
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="Q29" s="7">
         <v>0</v>
@@ -5785,15 +5648,15 @@
       </c>
       <c r="N30" s="7">
         <f>ROUND(income!$B$5 * $M30, 0)</f>
-        <v>145</v>
+        <v>0</v>
       </c>
       <c r="O30" s="7">
+        <f>ROUND(income!$F$5 * $M30, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P30" s="7">
         <f>ROUND(income!$C$5 * $M30, 0)</f>
-        <v>5</v>
-      </c>
-      <c r="P30" s="7">
-        <f>ROUND(income!$D$5 * $M30, 0)</f>
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="Q30" s="7">
         <v>0</v>
@@ -5831,15 +5694,15 @@
       </c>
       <c r="N31" s="7">
         <f>ROUND(income!$B$5 * $M31, 0)</f>
-        <v>152</v>
+        <v>0</v>
       </c>
       <c r="O31" s="7">
+        <f>ROUND(income!$F$5 * $M31, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P31" s="7">
         <f>ROUND(income!$C$5 * $M31, 0)</f>
-        <v>6</v>
-      </c>
-      <c r="P31" s="7">
-        <f>ROUND(income!$D$5 * $M31, 0)</f>
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="Q31" s="7">
         <v>0</v>
@@ -5877,15 +5740,15 @@
       </c>
       <c r="N32" s="7">
         <f>ROUND(income!$B$5 * $M32, 0)</f>
-        <v>159</v>
+        <v>0</v>
       </c>
       <c r="O32" s="7">
+        <f>ROUND(income!$F$5 * $M32, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P32" s="7">
         <f>ROUND(income!$C$5 * $M32, 0)</f>
-        <v>6</v>
-      </c>
-      <c r="P32" s="7">
-        <f>ROUND(income!$D$5 * $M32, 0)</f>
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="Q32" s="7">
         <v>0</v>
@@ -5923,15 +5786,15 @@
       </c>
       <c r="N33" s="7">
         <f>ROUND(income!$B$5 * $M33, 0)</f>
-        <v>166</v>
+        <v>0</v>
       </c>
       <c r="O33" s="7">
+        <f>ROUND(income!$F$5 * $M33, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P33" s="7">
         <f>ROUND(income!$C$5 * $M33, 0)</f>
-        <v>6</v>
-      </c>
-      <c r="P33" s="7">
-        <f>ROUND(income!$D$5 * $M33, 0)</f>
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="Q33" s="7">
         <v>0</v>
@@ -5972,15 +5835,15 @@
       </c>
       <c r="N34" s="7">
         <f>ROUND(income!$B$5 * $M34, 0)</f>
-        <v>248</v>
+        <v>0</v>
       </c>
       <c r="O34" s="7">
+        <f>ROUND(income!$F$5 * $M34, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P34" s="7">
         <f>ROUND(income!$C$5 * $M34, 0)</f>
-        <v>9</v>
-      </c>
-      <c r="P34" s="7">
-        <f>ROUND(income!$D$5 * $M34, 0)</f>
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="Q34" s="7">
         <v>0</v>
@@ -6022,15 +5885,15 @@
       </c>
       <c r="N35" s="7">
         <f>ROUND(income!$B$5 * $M35, 0)</f>
-        <v>262</v>
+        <v>0</v>
       </c>
       <c r="O35" s="7">
+        <f>ROUND(income!$F$5 * $M35, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P35" s="7">
         <f>ROUND(income!$C$5 * $M35, 0)</f>
-        <v>10</v>
-      </c>
-      <c r="P35" s="7">
-        <f>ROUND(income!$D$5 * $M35, 0)</f>
-        <v>74</v>
+        <v>0</v>
       </c>
       <c r="Q35" s="7">
         <v>0</v>
@@ -6072,15 +5935,15 @@
       </c>
       <c r="N36" s="7">
         <f>ROUND(income!$B$5 * $M36, 0)</f>
-        <v>276</v>
+        <v>0</v>
       </c>
       <c r="O36" s="7">
+        <f>ROUND(income!$F$5 * $M36, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P36" s="7">
         <f>ROUND(income!$C$5 * $M36, 0)</f>
-        <v>10</v>
-      </c>
-      <c r="P36" s="7">
-        <f>ROUND(income!$D$5 * $M36, 0)</f>
-        <v>78</v>
+        <v>0</v>
       </c>
       <c r="Q36" s="7">
         <v>0</v>
@@ -6122,15 +5985,15 @@
       </c>
       <c r="N37" s="7">
         <f>ROUND(income!$B$5 * $M37, 0)</f>
-        <v>290</v>
+        <v>0</v>
       </c>
       <c r="O37" s="7">
+        <f>ROUND(income!$F$5 * $M37, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P37" s="7">
         <f>ROUND(income!$C$5 * $M37, 0)</f>
-        <v>11</v>
-      </c>
-      <c r="P37" s="7">
-        <f>ROUND(income!$D$5 * $M37, 0)</f>
-        <v>82</v>
+        <v>0</v>
       </c>
       <c r="Q37" s="7">
         <v>0</v>
@@ -6171,19 +6034,19 @@
       <c r="K38" s="7"/>
       <c r="L38" s="7"/>
       <c r="M38" s="8">
-        <v>2.6</v>
+        <v>2.8</v>
       </c>
       <c r="N38" s="7">
         <f>ROUND(income!$B$5 * $M38, 0)</f>
-        <v>359</v>
+        <v>0</v>
       </c>
       <c r="O38" s="7">
+        <f>ROUND(income!$F$5 * $M38, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P38" s="7">
         <f>ROUND(income!$C$5 * $M38, 0)</f>
-        <v>13</v>
-      </c>
-      <c r="P38" s="7">
-        <f>ROUND(income!$D$5 * $M38, 0)</f>
-        <v>101</v>
+        <v>0</v>
       </c>
       <c r="Q38" s="7">
         <v>0</v>
@@ -6224,20 +6087,19 @@
       <c r="K39" s="7"/>
       <c r="L39" s="7"/>
       <c r="M39" s="8">
-        <f>M38+0.2</f>
-        <v>2.8000000000000003</v>
+        <v>3</v>
       </c>
       <c r="N39" s="7">
         <f>ROUND(income!$B$5 * $M39, 0)</f>
-        <v>386</v>
+        <v>0</v>
       </c>
       <c r="O39" s="7">
+        <f>ROUND(income!$F$5 * $M39, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P39" s="7">
         <f>ROUND(income!$C$5 * $M39, 0)</f>
-        <v>14</v>
-      </c>
-      <c r="P39" s="7">
-        <f>ROUND(income!$D$5 * $M39, 0)</f>
-        <v>109</v>
+        <v>0</v>
       </c>
       <c r="Q39" s="7">
         <v>0</v>
@@ -6279,19 +6141,19 @@
       <c r="L40" s="7"/>
       <c r="M40" s="8">
         <f>M39+0.2</f>
-        <v>3.0000000000000004</v>
+        <v>3.2</v>
       </c>
       <c r="N40" s="7">
         <f>ROUND(income!$B$5 * $M40, 0)</f>
-        <v>414</v>
+        <v>0</v>
       </c>
       <c r="O40" s="7">
+        <f>ROUND(income!$F$5 * $M40, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P40" s="7">
         <f>ROUND(income!$C$5 * $M40, 0)</f>
-        <v>15</v>
-      </c>
-      <c r="P40" s="7">
-        <f>ROUND(income!$D$5 * $M40, 0)</f>
-        <v>117</v>
+        <v>0</v>
       </c>
       <c r="Q40" s="7">
         <v>0</v>
@@ -6397,15 +6259,15 @@
       </c>
       <c r="N3" s="7">
         <f>ROUND(income!$B$3 * $M3, 0)</f>
-        <v>220</v>
+        <v>0</v>
       </c>
       <c r="O3" s="7">
+        <f>ROUND(income!$F$3 * $M3, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P3" s="7">
         <f>ROUND(income!$C$3 * $M3, 0)</f>
-        <v>8</v>
-      </c>
-      <c r="P3" s="7">
-        <f>ROUND(income!$D$3 * $M3, 0)</f>
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="Q3" s="7">
         <v>0</v>
@@ -6433,15 +6295,15 @@
       </c>
       <c r="N4" s="7">
         <f>ROUND(income!$B$3 * $M4, 0)</f>
-        <v>242</v>
+        <v>0</v>
       </c>
       <c r="O4" s="7">
+        <f>ROUND(income!$F$3 * $M4, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P4" s="7">
         <f>ROUND(income!$C$3 * $M4, 0)</f>
-        <v>9</v>
-      </c>
-      <c r="P4" s="7">
-        <f>ROUND(income!$D$3 * $M4, 0)</f>
-        <v>77</v>
+        <v>0</v>
       </c>
       <c r="Q4" s="7">
         <v>0</v>
@@ -6478,15 +6340,15 @@
       </c>
       <c r="N6" s="7">
         <f>ROUND(income!$B$4 * $M6, 0)</f>
-        <v>248</v>
+        <v>0</v>
       </c>
       <c r="O6" s="7">
+        <f>ROUND(income!$F$4 * $M6, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P6" s="7">
         <f>ROUND(income!$C$4 * $M6, 0)</f>
-        <v>8</v>
-      </c>
-      <c r="P6" s="7">
-        <f>ROUND(income!$D$4 * $M6, 0)</f>
-        <v>74</v>
+        <v>0</v>
       </c>
       <c r="Q6" s="7">
         <v>0</v>
@@ -6522,15 +6384,15 @@
       </c>
       <c r="N7" s="7">
         <f>ROUND(income!$B$4 * $M7, 0)</f>
-        <v>273</v>
+        <v>0</v>
       </c>
       <c r="O7" s="7">
+        <f>ROUND(income!$F$4 * $M7, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P7" s="7">
         <f>ROUND(income!$C$4 * $M7, 0)</f>
-        <v>9</v>
-      </c>
-      <c r="P7" s="7">
-        <f>ROUND(income!$D$4 * $M7, 0)</f>
-        <v>81</v>
+        <v>0</v>
       </c>
       <c r="Q7" s="7">
         <v>0</v>
@@ -6585,15 +6447,15 @@
       </c>
       <c r="N9" s="7">
         <f>ROUND(income!$B$5 * $M9, 0)</f>
-        <v>276</v>
+        <v>0</v>
       </c>
       <c r="O9" s="7">
+        <f>ROUND(income!$F$5 * $M9, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P9" s="7">
         <f>ROUND(income!$C$5 * $M9, 0)</f>
-        <v>10</v>
-      </c>
-      <c r="P9" s="7">
-        <f>ROUND(income!$D$5 * $M9, 0)</f>
-        <v>78</v>
+        <v>0</v>
       </c>
       <c r="Q9" s="7">
         <v>0</v>
@@ -6633,15 +6495,15 @@
       </c>
       <c r="N10" s="7">
         <f>ROUND(income!$B$5 * $M10, 0)</f>
-        <v>524</v>
+        <v>0</v>
       </c>
       <c r="O10" s="7">
+        <f>ROUND(income!$F$5 * $M10, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P10" s="7">
         <f>ROUND(income!$C$5 * $M10, 0)</f>
-        <v>19</v>
-      </c>
-      <c r="P10" s="7">
-        <f>ROUND(income!$D$5 * $M10, 0)</f>
-        <v>148</v>
+        <v>0</v>
       </c>
       <c r="Q10" s="7">
         <v>0</v>
@@ -6700,19 +6562,19 @@
       </c>
       <c r="N12" s="7">
         <f>ROUND(income!$B$6 * $M12, 0)</f>
-        <v>608</v>
+        <v>0</v>
       </c>
       <c r="O12" s="7">
+        <f>ROUND(income!$F$6 * $M12, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P12" s="7">
         <f>ROUND(income!$C$6 * $M12, 0)</f>
-        <v>20</v>
-      </c>
-      <c r="P12" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="7">
         <f>ROUND(income!$D$6 * $M12, 0)</f>
-        <v>164</v>
-      </c>
-      <c r="Q12" s="7">
-        <f>ROUND(income!$E$6 * $M12, 0)</f>
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="R12" s="7">
         <v>0</v>
@@ -6749,19 +6611,19 @@
       </c>
       <c r="N13" s="7">
         <f>ROUND(income!$B$6 * $M13, 0)</f>
-        <v>669</v>
+        <v>0</v>
       </c>
       <c r="O13" s="7">
+        <f>ROUND(income!$F$6 * $M13, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P13" s="7">
         <f>ROUND(income!$C$6 * $M13, 0)</f>
-        <v>22</v>
-      </c>
-      <c r="P13" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="7">
         <f>ROUND(income!$D$6 * $M13, 0)</f>
-        <v>180</v>
-      </c>
-      <c r="Q13" s="7">
-        <f>ROUND(income!$E$6 * $M13, 0)</f>
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="R13" s="7">
         <v>0</v>
@@ -6817,19 +6679,19 @@
       </c>
       <c r="N15" s="7">
         <f>ROUND(income!$B$7 * $M15, 0)</f>
-        <v>664</v>
+        <v>0</v>
       </c>
       <c r="O15" s="7">
+        <f>ROUND(income!$F$7 * $M15, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P15" s="7">
         <f>ROUND(income!$C$7 * $M15, 0)</f>
-        <v>24</v>
-      </c>
-      <c r="P15" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="7">
         <f>ROUND(income!$D$7 * $M15, 0)</f>
-        <v>172</v>
-      </c>
-      <c r="Q15" s="7">
-        <f>ROUND(income!$E$7 * $M15, 0)</f>
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="R15" s="7">
         <v>0</v>
@@ -6866,19 +6728,19 @@
       </c>
       <c r="N16" s="7">
         <f>ROUND(income!$B$7 * $M16, 0)</f>
-        <v>730</v>
+        <v>0</v>
       </c>
       <c r="O16" s="7">
+        <f>ROUND(income!$F$7 * $M16, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P16" s="7">
         <f>ROUND(income!$C$7 * $M16, 0)</f>
-        <v>26</v>
-      </c>
-      <c r="P16" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="7">
         <f>ROUND(income!$D$7 * $M16, 0)</f>
-        <v>189</v>
-      </c>
-      <c r="Q16" s="7">
-        <f>ROUND(income!$E$7 * $M16, 0)</f>
-        <v>97</v>
+        <v>0</v>
       </c>
       <c r="R16" s="7">
         <v>0</v>
@@ -6918,19 +6780,19 @@
       </c>
       <c r="N18" s="7">
         <f>ROUND(income!$B$8 * $M18, 0)</f>
-        <v>720</v>
+        <v>0</v>
       </c>
       <c r="O18" s="7">
+        <f>ROUND(income!$F$8 * $M18, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P18" s="7">
         <f>ROUND(income!$C$8 * $M18, 0)</f>
-        <v>24</v>
-      </c>
-      <c r="P18" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="7">
         <f>ROUND(income!$D$8 * $M18, 0)</f>
-        <v>180</v>
-      </c>
-      <c r="Q18" s="7">
-        <f>ROUND(income!$E$8 * $M18, 0)</f>
-        <v>96</v>
+        <v>0</v>
       </c>
       <c r="R18" s="7">
         <v>0</v>
@@ -6969,19 +6831,19 @@
       </c>
       <c r="N19" s="7">
         <f>ROUND(income!$B$8 * $M19, 0)</f>
-        <v>1008</v>
+        <v>0</v>
       </c>
       <c r="O19" s="7">
+        <f>ROUND(income!$F$8 * $M19, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P19" s="7">
         <f>ROUND(income!$C$8 * $M19, 0)</f>
-        <v>34</v>
-      </c>
-      <c r="P19" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="7">
         <f>ROUND(income!$D$8 * $M19, 0)</f>
-        <v>252</v>
-      </c>
-      <c r="Q19" s="7">
-        <f>ROUND(income!$E$8 * $M19, 0)</f>
-        <v>134</v>
+        <v>0</v>
       </c>
       <c r="R19" s="7">
         <v>0</v>
@@ -7433,15 +7295,15 @@
       </c>
       <c r="N3" s="7">
         <f>ROUND(income!B$3 * $M3, 0)</f>
-        <v>330</v>
+        <v>0</v>
       </c>
       <c r="O3" s="7">
+        <f>ROUND(income!F$3 * $M3, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P3" s="7">
         <f>ROUND(income!C$3 * $M3, 0)</f>
-        <v>12</v>
-      </c>
-      <c r="P3" s="7">
-        <f>ROUND(income!D$3 * $M3, 0)</f>
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="Q3" s="7">
         <v>0</v>
@@ -7504,15 +7366,15 @@
       </c>
       <c r="N5" s="7">
         <f>ROUND(income!$B$4 * $M5, 0)</f>
-        <v>384</v>
+        <v>0</v>
       </c>
       <c r="O5" s="7">
+        <f>ROUND(income!$F$4 * $M5, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P5" s="7">
         <f>ROUND(income!$C$4 * $M5, 0)</f>
-        <v>12</v>
-      </c>
-      <c r="P5" s="7">
-        <f>ROUND(income!$D$4 * $M5, 0)</f>
-        <v>115</v>
+        <v>0</v>
       </c>
       <c r="Q5" s="7">
         <v>0</v>
@@ -7579,15 +7441,15 @@
       </c>
       <c r="N7" s="7">
         <f>ROUND(income!$B$5 * $M7, 0)</f>
-        <v>442</v>
+        <v>0</v>
       </c>
       <c r="O7" s="7">
+        <f>ROUND(income!$F$5 * $M7, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P7" s="7">
         <f>ROUND(income!$C$5 * $M7, 0)</f>
-        <v>16</v>
-      </c>
-      <c r="P7" s="7">
-        <f>ROUND(income!$D$5 * $M7, 0)</f>
-        <v>125</v>
+        <v>0</v>
       </c>
       <c r="Q7" s="7">
         <v>0</v>
@@ -7654,19 +7516,19 @@
       </c>
       <c r="N9" s="7">
         <f>ROUND(income!$B$6 * $M9, 0)</f>
-        <v>502</v>
+        <v>0</v>
       </c>
       <c r="O9" s="7">
+        <f>ROUND(income!$F$6 * $M9, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P9" s="7">
         <f>ROUND(income!$C$6 * $M9, 0)</f>
-        <v>17</v>
-      </c>
-      <c r="P9" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="7">
         <f>ROUND(income!$D$6 * $M9, 0)</f>
-        <v>135</v>
-      </c>
-      <c r="Q9" s="7">
-        <f>ROUND(income!$E$6 * $M9, 0)</f>
-        <v>66</v>
+        <v>0</v>
       </c>
       <c r="R9" s="7">
         <v>0</v>
@@ -7730,19 +7592,19 @@
       </c>
       <c r="N11" s="7">
         <f>ROUND(income!$B$7 * $M11, 0)</f>
-        <v>564</v>
+        <v>0</v>
       </c>
       <c r="O11" s="7">
+        <f>ROUND(income!$F$7 * $M11, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P11" s="7">
         <f>ROUND(income!$C$7 * $M11, 0)</f>
-        <v>20</v>
-      </c>
-      <c r="P11" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="7">
         <f>ROUND(income!$D$7 * $M11, 0)</f>
-        <v>146</v>
-      </c>
-      <c r="Q11" s="7">
-        <f>ROUND(income!$E$7 * $M11, 0)</f>
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="R11" s="7">
         <v>0</v>
@@ -7802,19 +7664,19 @@
       </c>
       <c r="N13" s="7">
         <f>ROUND(income!$B$8 * $M13, 0)</f>
-        <v>630</v>
+        <v>0</v>
       </c>
       <c r="O13" s="7">
+        <f>ROUND(income!$F$8 * $M13, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P13" s="7">
         <f>ROUND(income!$C$8 * $M13, 0)</f>
-        <v>21</v>
-      </c>
-      <c r="P13" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="7">
         <f>ROUND(income!$D$8 * $M13, 0)</f>
-        <v>158</v>
-      </c>
-      <c r="Q13" s="7">
-        <f>ROUND(income!$E$8 * $M13, 0)</f>
-        <v>84</v>
+        <v>0</v>
       </c>
       <c r="R13" s="7">
         <v>0</v>
@@ -7848,23 +7710,23 @@
       </c>
       <c r="N15" s="7">
         <f>ROUND(income!B$9 * $M15, 0)</f>
-        <v>698</v>
+        <v>0</v>
       </c>
       <c r="O15" s="7">
+        <f>ROUND(income!F$9 * $M15, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P15" s="7">
         <f>ROUND(income!C$9 * $M15, 0)</f>
-        <v>25</v>
-      </c>
-      <c r="P15" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="7">
         <f>ROUND(income!D$9 * $M15, 0)</f>
-        <v>169</v>
-      </c>
-      <c r="Q15" s="7">
+        <v>0</v>
+      </c>
+      <c r="R15" s="7">
         <f>ROUND(income!E$9 * $M15, 0)</f>
-        <v>94</v>
-      </c>
-      <c r="R15" s="7">
-        <f>ROUND(income!F$9 * $M15, 0)</f>
-        <v>47</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -7897,23 +7759,23 @@
       </c>
       <c r="N17" s="7">
         <f>ROUND(income!B$10 * $M17, 0)</f>
-        <v>770</v>
+        <v>0</v>
       </c>
       <c r="O17" s="7">
+        <f>ROUND(income!F$10 * $M17, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P17" s="7">
         <f>ROUND(income!C$10 * $M17, 0)</f>
-        <v>26</v>
-      </c>
-      <c r="P17" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="7">
         <f>ROUND(income!D$10 * $M17, 0)</f>
-        <v>181</v>
-      </c>
-      <c r="Q17" s="7">
+        <v>0</v>
+      </c>
+      <c r="R17" s="7">
         <f>ROUND(income!E$10 * $M17, 0)</f>
-        <v>104</v>
-      </c>
-      <c r="R17" s="7">
-        <f>ROUND(income!F$10 * $M17, 0)</f>
-        <v>52</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -7946,23 +7808,23 @@
       </c>
       <c r="N19" s="7">
         <f>ROUND(income!B$11 * $M19, 0)</f>
-        <v>844</v>
+        <v>0</v>
       </c>
       <c r="O19" s="7">
+        <f>ROUND(income!F$11 * $M19, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P19" s="7">
         <f>ROUND(income!C$11 * $M19, 0)</f>
-        <v>30</v>
-      </c>
-      <c r="P19" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="7">
         <f>ROUND(income!D$11 * $M19, 0)</f>
-        <v>194</v>
-      </c>
-      <c r="Q19" s="7">
+        <v>0</v>
+      </c>
+      <c r="R19" s="7">
         <f>ROUND(income!E$11 * $M19, 0)</f>
-        <v>114</v>
-      </c>
-      <c r="R19" s="7">
-        <f>ROUND(income!F$11 * $M19, 0)</f>
-        <v>57</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -8142,15 +8004,15 @@
       </c>
       <c r="N3" s="7">
         <f>ROUND(income!$B$3 * $M3, 0)</f>
-        <v>440</v>
+        <v>0</v>
       </c>
       <c r="O3" s="7">
+        <f>ROUND(income!$F$3 * $M3, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P3" s="7">
         <f>ROUND(income!$C$3 * $M3, 0)</f>
-        <v>16</v>
-      </c>
-      <c r="P3" s="7">
-        <f>ROUND(income!$D$3 * $M3, 0)</f>
-        <v>140</v>
+        <v>0</v>
       </c>
       <c r="Q3" s="7">
         <v>0</v>
@@ -8180,15 +8042,15 @@
       </c>
       <c r="N4" s="7">
         <f>ROUND(income!$B$3 * M4, 0)</f>
-        <v>446</v>
+        <v>0</v>
       </c>
       <c r="O4" s="7">
+        <f>ROUND(income!$F$3 * $M4, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P4" s="7">
         <f>ROUND(income!$C$3 * $M4, 0)</f>
-        <v>16</v>
-      </c>
-      <c r="P4" s="7">
-        <f>ROUND(income!$D$3 * $M4, 0)</f>
-        <v>142</v>
+        <v>0</v>
       </c>
       <c r="Q4" s="7">
         <v>0</v>
@@ -8218,15 +8080,15 @@
       </c>
       <c r="N5" s="7">
         <f>ROUND(income!$B$3 * M5, 0)</f>
-        <v>451</v>
+        <v>0</v>
       </c>
       <c r="O5" s="7">
+        <f>ROUND(income!$F$3 * $M5, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P5" s="7">
         <f>ROUND(income!$C$3 * $M5, 0)</f>
-        <v>16</v>
-      </c>
-      <c r="P5" s="7">
-        <f>ROUND(income!$D$3 * $M5, 0)</f>
-        <v>144</v>
+        <v>0</v>
       </c>
       <c r="Q5" s="7">
         <v>0</v>
@@ -8256,15 +8118,15 @@
       </c>
       <c r="N6" s="7">
         <f>ROUND(income!$B$3 * M6, 0)</f>
-        <v>457</v>
+        <v>0</v>
       </c>
       <c r="O6" s="7">
+        <f>ROUND(income!$F$3 * $M6, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P6" s="7">
         <f>ROUND(income!$C$3 * $M6, 0)</f>
-        <v>17</v>
-      </c>
-      <c r="P6" s="7">
-        <f>ROUND(income!$D$3 * $M6, 0)</f>
-        <v>145</v>
+        <v>0</v>
       </c>
       <c r="Q6" s="7">
         <v>0</v>
@@ -8300,15 +8162,15 @@
       </c>
       <c r="N7" s="7">
         <f>ROUND(income!$B$3 * M7, 0)</f>
-        <v>462</v>
+        <v>0</v>
       </c>
       <c r="O7" s="7">
+        <f>ROUND(income!$F$3 * $M7, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P7" s="7">
         <f>ROUND(income!$C$3 * $M7, 0)</f>
-        <v>17</v>
-      </c>
-      <c r="P7" s="7">
-        <f>ROUND(income!$D$3 * $M7, 0)</f>
-        <v>147</v>
+        <v>0</v>
       </c>
       <c r="Q7" s="7">
         <v>0</v>
@@ -8344,15 +8206,15 @@
       </c>
       <c r="N8" s="7">
         <f>ROUND(income!$B$3 * M8, 0)</f>
-        <v>468</v>
+        <v>0</v>
       </c>
       <c r="O8" s="7">
+        <f>ROUND(income!$F$3 * $M8, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P8" s="7">
         <f>ROUND(income!$C$3 * $M8, 0)</f>
-        <v>17</v>
-      </c>
-      <c r="P8" s="7">
-        <f>ROUND(income!$D$3 * $M8, 0)</f>
-        <v>149</v>
+        <v>0</v>
       </c>
       <c r="Q8" s="7">
         <v>0</v>
@@ -8388,15 +8250,15 @@
       </c>
       <c r="N9" s="7">
         <f>ROUND(income!$B$3 * M9, 0)</f>
-        <v>473</v>
+        <v>0</v>
       </c>
       <c r="O9" s="7">
+        <f>ROUND(income!$F$3 * $M9, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P9" s="7">
         <f>ROUND(income!$C$3 * $M9, 0)</f>
-        <v>17</v>
-      </c>
-      <c r="P9" s="7">
-        <f>ROUND(income!$D$3 * $M9, 0)</f>
-        <v>151</v>
+        <v>0</v>
       </c>
       <c r="Q9" s="7">
         <v>0</v>
@@ -8432,15 +8294,15 @@
       </c>
       <c r="N10" s="7">
         <f>ROUND(income!$B$3 * M10, 0)</f>
-        <v>479</v>
+        <v>0</v>
       </c>
       <c r="O10" s="7">
+        <f>ROUND(income!$F$3 * $M10, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P10" s="7">
         <f>ROUND(income!$C$3 * $M10, 0)</f>
-        <v>17</v>
-      </c>
-      <c r="P10" s="7">
-        <f>ROUND(income!$D$3 * $M10, 0)</f>
-        <v>152</v>
+        <v>0</v>
       </c>
       <c r="Q10" s="7">
         <v>0</v>
@@ -8482,15 +8344,15 @@
       </c>
       <c r="N11" s="7">
         <f>ROUND(income!$B$3 * M11, 0)</f>
-        <v>484</v>
+        <v>0</v>
       </c>
       <c r="O11" s="7">
+        <f>ROUND(income!$F$3 * $M11, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P11" s="7">
         <f>ROUND(income!$C$3 * $M11, 0)</f>
-        <v>18</v>
-      </c>
-      <c r="P11" s="7">
-        <f>ROUND(income!$D$3 * $M11, 0)</f>
-        <v>154</v>
+        <v>0</v>
       </c>
       <c r="Q11" s="7">
         <v>0</v>
@@ -8532,15 +8394,15 @@
       </c>
       <c r="N12" s="7">
         <f>ROUND(income!$B$3 * M12, 0)</f>
-        <v>490</v>
+        <v>0</v>
       </c>
       <c r="O12" s="7">
+        <f>ROUND(income!$F$3 * $M12, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P12" s="7">
         <f>ROUND(income!$C$3 * $M12, 0)</f>
-        <v>18</v>
-      </c>
-      <c r="P12" s="7">
-        <f>ROUND(income!$D$3 * $M12, 0)</f>
-        <v>156</v>
+        <v>0</v>
       </c>
       <c r="Q12" s="7">
         <v>0</v>
@@ -8585,15 +8447,15 @@
       </c>
       <c r="N14" s="7">
         <f>ROUND(income!$B$4 * $M14, 0)</f>
-        <v>496</v>
+        <v>0</v>
       </c>
       <c r="O14" s="7">
+        <f>ROUND(income!$F$4 * $M14, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P14" s="7">
         <f>ROUND(income!$C$4 * $M14, 0)</f>
-        <v>16</v>
-      </c>
-      <c r="P14" s="7">
-        <f>ROUND(income!$D$4 * $M14, 0)</f>
-        <v>148</v>
+        <v>0</v>
       </c>
       <c r="Q14" s="7">
         <v>0</v>
@@ -8623,15 +8485,15 @@
       </c>
       <c r="N15" s="7">
         <f>ROUND(income!$B$4 * $M15, 0)</f>
-        <v>502</v>
+        <v>0</v>
       </c>
       <c r="O15" s="7">
+        <f>ROUND(income!$F$4 * $M15, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P15" s="7">
         <f>ROUND(income!$C$4 * $M15, 0)</f>
-        <v>16</v>
-      </c>
-      <c r="P15" s="7">
-        <f>ROUND(income!$D$4 * $M15, 0)</f>
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="Q15" s="7">
         <v>0</v>
@@ -8661,15 +8523,15 @@
       </c>
       <c r="N16" s="7">
         <f>ROUND(income!$B$4 * $M16, 0)</f>
-        <v>508</v>
+        <v>0</v>
       </c>
       <c r="O16" s="7">
+        <f>ROUND(income!$F$4 * $M16, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P16" s="7">
         <f>ROUND(income!$C$4 * $M16, 0)</f>
-        <v>16</v>
-      </c>
-      <c r="P16" s="7">
-        <f>ROUND(income!$D$4 * $M16, 0)</f>
-        <v>152</v>
+        <v>0</v>
       </c>
       <c r="Q16" s="7">
         <v>0</v>
@@ -8705,15 +8567,15 @@
       </c>
       <c r="N17" s="7">
         <f>ROUND(income!$B$4 * $M17, 0)</f>
-        <v>515</v>
+        <v>0</v>
       </c>
       <c r="O17" s="7">
+        <f>ROUND(income!$F$4 * $M17, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P17" s="7">
         <f>ROUND(income!$C$4 * $M17, 0)</f>
-        <v>17</v>
-      </c>
-      <c r="P17" s="7">
-        <f>ROUND(income!$D$4 * $M17, 0)</f>
-        <v>154</v>
+        <v>0</v>
       </c>
       <c r="Q17" s="7">
         <v>0</v>
@@ -8749,15 +8611,15 @@
       </c>
       <c r="N18" s="7">
         <f>ROUND(income!$B$4 * $M18, 0)</f>
-        <v>521</v>
+        <v>0</v>
       </c>
       <c r="O18" s="7">
+        <f>ROUND(income!$F$4 * $M18, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P18" s="7">
         <f>ROUND(income!$C$4 * $M18, 0)</f>
-        <v>17</v>
-      </c>
-      <c r="P18" s="7">
-        <f>ROUND(income!$D$4 * $M18, 0)</f>
-        <v>155</v>
+        <v>0</v>
       </c>
       <c r="Q18" s="7">
         <v>0</v>
@@ -8787,15 +8649,15 @@
       </c>
       <c r="N19" s="7">
         <f>ROUND(income!$B$4 * $M19, 0)</f>
-        <v>527</v>
+        <v>0</v>
       </c>
       <c r="O19" s="7">
+        <f>ROUND(income!$F$4 * $M19, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P19" s="7">
         <f>ROUND(income!$C$4 * $M19, 0)</f>
-        <v>17</v>
-      </c>
-      <c r="P19" s="7">
-        <f>ROUND(income!$D$4 * $M19, 0)</f>
-        <v>157</v>
+        <v>0</v>
       </c>
       <c r="Q19" s="7">
         <v>0</v>
@@ -8831,15 +8693,15 @@
       </c>
       <c r="N20" s="7">
         <f>ROUND(income!$B$4 * $M20, 0)</f>
-        <v>533</v>
+        <v>0</v>
       </c>
       <c r="O20" s="7">
+        <f>ROUND(income!$F$4 * $M20, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P20" s="7">
         <f>ROUND(income!$C$4 * $M20, 0)</f>
-        <v>17</v>
-      </c>
-      <c r="P20" s="7">
-        <f>ROUND(income!$D$4 * $M20, 0)</f>
-        <v>159</v>
+        <v>0</v>
       </c>
       <c r="Q20" s="7">
         <v>0</v>
@@ -8875,15 +8737,15 @@
       </c>
       <c r="N21" s="7">
         <f>ROUND(income!$B$4 * $M21, 0)</f>
-        <v>539</v>
+        <v>0</v>
       </c>
       <c r="O21" s="7">
+        <f>ROUND(income!$F$4 * $M21, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P21" s="7">
         <f>ROUND(income!$C$4 * $M21, 0)</f>
-        <v>17</v>
-      </c>
-      <c r="P21" s="7">
-        <f>ROUND(income!$D$4 * $M21, 0)</f>
-        <v>161</v>
+        <v>0</v>
       </c>
       <c r="Q21" s="7">
         <v>0</v>
@@ -8913,15 +8775,15 @@
       </c>
       <c r="N22" s="7">
         <f>ROUND(income!$B$4 * $M22, 0)</f>
-        <v>546</v>
+        <v>0</v>
       </c>
       <c r="O22" s="7">
+        <f>ROUND(income!$F$4 * $M22, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P22" s="7">
         <f>ROUND(income!$C$4 * $M22, 0)</f>
-        <v>18</v>
-      </c>
-      <c r="P22" s="7">
-        <f>ROUND(income!$D$4 * $M22, 0)</f>
-        <v>163</v>
+        <v>0</v>
       </c>
       <c r="Q22" s="7">
         <v>0</v>
@@ -8957,15 +8819,15 @@
       </c>
       <c r="N23" s="7">
         <f>ROUND(income!$B$4 * $M23, 0)</f>
-        <v>552</v>
+        <v>0</v>
       </c>
       <c r="O23" s="7">
+        <f>ROUND(income!$F$4 * $M23, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P23" s="7">
         <f>ROUND(income!$C$4 * $M23, 0)</f>
-        <v>18</v>
-      </c>
-      <c r="P23" s="7">
-        <f>ROUND(income!$D$4 * $M23, 0)</f>
-        <v>165</v>
+        <v>0</v>
       </c>
       <c r="Q23" s="7">
         <v>0</v>
@@ -9001,15 +8863,15 @@
       </c>
       <c r="N24" s="7">
         <f>ROUND(income!$B$4 * $M24, 0)</f>
-        <v>558</v>
+        <v>0</v>
       </c>
       <c r="O24" s="7">
+        <f>ROUND(income!$F$4 * $M24, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P24" s="7">
         <f>ROUND(income!$C$4 * $M24, 0)</f>
-        <v>18</v>
-      </c>
-      <c r="P24" s="7">
-        <f>ROUND(income!$D$4 * $M24, 0)</f>
-        <v>167</v>
+        <v>0</v>
       </c>
       <c r="Q24" s="7">
         <v>0</v>
@@ -9039,15 +8901,15 @@
       </c>
       <c r="N25" s="7">
         <f>ROUND(income!$B$4 * $M25, 0)</f>
-        <v>564</v>
+        <v>0</v>
       </c>
       <c r="O25" s="7">
+        <f>ROUND(income!$F$4 * $M25, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P25" s="7">
         <f>ROUND(income!$C$4 * $M25, 0)</f>
-        <v>18</v>
-      </c>
-      <c r="P25" s="7">
-        <f>ROUND(income!$D$4 * $M25, 0)</f>
-        <v>168</v>
+        <v>0</v>
       </c>
       <c r="Q25" s="7">
         <v>0</v>
@@ -9089,15 +8951,15 @@
       </c>
       <c r="N26" s="7">
         <f>ROUND(income!$B$4 * $M26, 0)</f>
-        <v>570</v>
+        <v>0</v>
       </c>
       <c r="O26" s="7">
+        <f>ROUND(income!$F$4 * $M26, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P26" s="7">
         <f>ROUND(income!$C$4 * $M26, 0)</f>
-        <v>18</v>
-      </c>
-      <c r="P26" s="7">
-        <f>ROUND(income!$D$4 * $M26, 0)</f>
-        <v>170</v>
+        <v>0</v>
       </c>
       <c r="Q26" s="7">
         <v>0</v>
@@ -9139,15 +9001,15 @@
       </c>
       <c r="N27" s="7">
         <f>ROUND(income!$B$4 * $M27, 0)</f>
-        <v>577</v>
+        <v>0</v>
       </c>
       <c r="O27" s="7">
+        <f>ROUND(income!$F$4 * $M27, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P27" s="7">
         <f>ROUND(income!$C$4 * $M27, 0)</f>
-        <v>19</v>
-      </c>
-      <c r="P27" s="7">
-        <f>ROUND(income!$D$4 * $M27, 0)</f>
-        <v>172</v>
+        <v>0</v>
       </c>
       <c r="Q27" s="7">
         <v>0</v>
@@ -9179,15 +9041,15 @@
       </c>
       <c r="N29" s="7">
         <f>ROUND(income!$B$5 * $M29, 0)</f>
-        <v>552</v>
+        <v>0</v>
       </c>
       <c r="O29" s="7">
+        <f>ROUND(income!$F$5 * $M29, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P29" s="7">
         <f>ROUND(income!$C$5 * $M29, 0)</f>
-        <v>20</v>
-      </c>
-      <c r="P29" s="7">
-        <f>ROUND(income!$D$5 * $M29, 0)</f>
-        <v>156</v>
+        <v>0</v>
       </c>
       <c r="Q29" s="7">
         <v>0</v>
@@ -9217,15 +9079,15 @@
       </c>
       <c r="N30" s="7">
         <f>ROUND(income!$B$5 * $M30, 0)</f>
-        <v>559</v>
+        <v>0</v>
       </c>
       <c r="O30" s="7">
+        <f>ROUND(income!$F$5 * $M30, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P30" s="7">
         <f>ROUND(income!$C$5 * $M30, 0)</f>
-        <v>20</v>
-      </c>
-      <c r="P30" s="7">
-        <f>ROUND(income!$D$5 * $M30, 0)</f>
-        <v>158</v>
+        <v>0</v>
       </c>
       <c r="Q30" s="7">
         <v>0</v>
@@ -9255,15 +9117,15 @@
       </c>
       <c r="N31" s="7">
         <f>ROUND(income!$B$5 * $M31, 0)</f>
-        <v>566</v>
+        <v>0</v>
       </c>
       <c r="O31" s="7">
+        <f>ROUND(income!$F$5 * $M31, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P31" s="7">
         <f>ROUND(income!$C$5 * $M31, 0)</f>
-        <v>21</v>
-      </c>
-      <c r="P31" s="7">
-        <f>ROUND(income!$D$5 * $M31, 0)</f>
-        <v>160</v>
+        <v>0</v>
       </c>
       <c r="Q31" s="7">
         <v>0</v>
@@ -9299,15 +9161,15 @@
       </c>
       <c r="N32" s="7">
         <f>ROUND(income!$B$5 * $M32, 0)</f>
-        <v>573</v>
+        <v>0</v>
       </c>
       <c r="O32" s="7">
+        <f>ROUND(income!$F$5 * $M32, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P32" s="7">
         <f>ROUND(income!$C$5 * $M32, 0)</f>
-        <v>21</v>
-      </c>
-      <c r="P32" s="7">
-        <f>ROUND(income!$D$5 * $M32, 0)</f>
-        <v>162</v>
+        <v>0</v>
       </c>
       <c r="Q32" s="7">
         <v>0</v>
@@ -9337,15 +9199,15 @@
       </c>
       <c r="N33" s="7">
         <f>ROUND(income!$B$5 * $M33, 0)</f>
-        <v>580</v>
+        <v>0</v>
       </c>
       <c r="O33" s="7">
+        <f>ROUND(income!$F$5 * $M33, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P33" s="7">
         <f>ROUND(income!$C$5 * $M33, 0)</f>
-        <v>21</v>
-      </c>
-      <c r="P33" s="7">
-        <f>ROUND(income!$D$5 * $M33, 0)</f>
-        <v>164</v>
+        <v>0</v>
       </c>
       <c r="Q33" s="7">
         <v>0</v>
@@ -9381,15 +9243,15 @@
       </c>
       <c r="N34" s="7">
         <f>ROUND(income!$B$5 * $M34, 0)</f>
-        <v>587</v>
+        <v>0</v>
       </c>
       <c r="O34" s="7">
+        <f>ROUND(income!$F$5 * $M34, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P34" s="7">
         <f>ROUND(income!$C$5 * $M34, 0)</f>
-        <v>21</v>
-      </c>
-      <c r="P34" s="7">
-        <f>ROUND(income!$D$5 * $M34, 0)</f>
-        <v>166</v>
+        <v>0</v>
       </c>
       <c r="Q34" s="7">
         <v>0</v>
@@ -9425,15 +9287,15 @@
       </c>
       <c r="N35" s="7">
         <f>ROUND(income!$B$5 * $M35, 0)</f>
-        <v>593</v>
+        <v>0</v>
       </c>
       <c r="O35" s="7">
+        <f>ROUND(income!$F$5 * $M35, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P35" s="7">
         <f>ROUND(income!$C$5 * $M35, 0)</f>
-        <v>22</v>
-      </c>
-      <c r="P35" s="7">
-        <f>ROUND(income!$D$5 * $M35, 0)</f>
-        <v>168</v>
+        <v>0</v>
       </c>
       <c r="Q35" s="7">
         <v>0</v>
@@ -9469,15 +9331,15 @@
       </c>
       <c r="N36" s="7">
         <f>ROUND(income!$B$5 * $M36, 0)</f>
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="O36" s="7">
+        <f>ROUND(income!$F$5 * $M36, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P36" s="7">
         <f>ROUND(income!$C$5 * $M36, 0)</f>
-        <v>22</v>
-      </c>
-      <c r="P36" s="7">
-        <f>ROUND(income!$D$5 * $M36, 0)</f>
-        <v>170</v>
+        <v>0</v>
       </c>
       <c r="Q36" s="7">
         <v>0</v>
@@ -9513,15 +9375,15 @@
       </c>
       <c r="N37" s="7">
         <f>ROUND(income!$B$5 * $M37, 0)</f>
-        <v>607</v>
+        <v>0</v>
       </c>
       <c r="O37" s="7">
+        <f>ROUND(income!$F$5 * $M37, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P37" s="7">
         <f>ROUND(income!$C$5 * $M37, 0)</f>
-        <v>22</v>
-      </c>
-      <c r="P37" s="7">
-        <f>ROUND(income!$D$5 * $M37, 0)</f>
-        <v>172</v>
+        <v>0</v>
       </c>
       <c r="Q37" s="7">
         <v>0</v>
@@ -9563,15 +9425,15 @@
       </c>
       <c r="N38" s="7">
         <f>ROUND(income!$B$5 * $M38, 0)</f>
-        <v>614</v>
+        <v>0</v>
       </c>
       <c r="O38" s="7">
+        <f>ROUND(income!$F$5 * $M38, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P38" s="7">
         <f>ROUND(income!$C$5 * $M38, 0)</f>
-        <v>22</v>
-      </c>
-      <c r="P38" s="7">
-        <f>ROUND(income!$D$5 * $M38, 0)</f>
-        <v>174</v>
+        <v>0</v>
       </c>
       <c r="Q38" s="7">
         <v>0</v>
@@ -9607,15 +9469,15 @@
       </c>
       <c r="N39" s="7">
         <f>ROUND(income!$B$5 * $M39, 0)</f>
-        <v>621</v>
+        <v>0</v>
       </c>
       <c r="O39" s="7">
+        <f>ROUND(income!$F$5 * $M39, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P39" s="7">
         <f>ROUND(income!$C$5 * $M39, 0)</f>
-        <v>23</v>
-      </c>
-      <c r="P39" s="7">
-        <f>ROUND(income!$D$5 * $M39, 0)</f>
-        <v>176</v>
+        <v>0</v>
       </c>
       <c r="Q39" s="7">
         <v>0</v>
@@ -9651,15 +9513,15 @@
       </c>
       <c r="N40" s="7">
         <f>ROUND(income!$B$5 * $M40, 0)</f>
-        <v>628</v>
+        <v>0</v>
       </c>
       <c r="O40" s="7">
+        <f>ROUND(income!$F$5 * $M40, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P40" s="7">
         <f>ROUND(income!$C$5 * $M40, 0)</f>
-        <v>23</v>
-      </c>
-      <c r="P40" s="7">
-        <f>ROUND(income!$D$5 * $M40, 0)</f>
-        <v>177</v>
+        <v>0</v>
       </c>
       <c r="Q40" s="7">
         <v>0</v>
@@ -9695,15 +9557,15 @@
       </c>
       <c r="N41" s="7">
         <f>ROUND(income!$B$5 * $M41, 0)</f>
-        <v>635</v>
+        <v>0</v>
       </c>
       <c r="O41" s="7">
+        <f>ROUND(income!$F$5 * $M41, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P41" s="7">
         <f>ROUND(income!$C$5 * $M41, 0)</f>
-        <v>23</v>
-      </c>
-      <c r="P41" s="7">
-        <f>ROUND(income!$D$5 * $M41, 0)</f>
-        <v>179</v>
+        <v>0</v>
       </c>
       <c r="Q41" s="7">
         <v>0</v>
@@ -9745,15 +9607,15 @@
       </c>
       <c r="N42" s="7">
         <f>ROUND(income!$B$5 * $M42, 0)</f>
-        <v>642</v>
+        <v>0</v>
       </c>
       <c r="O42" s="7">
+        <f>ROUND(income!$F$5 * $M42, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P42" s="7">
         <f>ROUND(income!$C$5 * $M42, 0)</f>
-        <v>23</v>
-      </c>
-      <c r="P42" s="7">
-        <f>ROUND(income!$D$5 * $M42, 0)</f>
-        <v>181</v>
+        <v>0</v>
       </c>
       <c r="Q42" s="7">
         <v>0</v>
@@ -9789,15 +9651,15 @@
       </c>
       <c r="N43" s="7">
         <f>ROUND(income!$B$5 * $M43, 0)</f>
-        <v>649</v>
+        <v>0</v>
       </c>
       <c r="O43" s="7">
+        <f>ROUND(income!$F$5 * $M43, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P43" s="7">
         <f>ROUND(income!$C$5 * $M43, 0)</f>
-        <v>24</v>
-      </c>
-      <c r="P43" s="7">
-        <f>ROUND(income!$D$5 * $M43, 0)</f>
-        <v>183</v>
+        <v>0</v>
       </c>
       <c r="Q43" s="7">
         <v>0</v>
@@ -9839,15 +9701,15 @@
       </c>
       <c r="N44" s="7">
         <f>ROUND(income!$B$5 * $M44, 0)</f>
-        <v>656</v>
+        <v>0</v>
       </c>
       <c r="O44" s="7">
+        <f>ROUND(income!$F$5 * $M44, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P44" s="7">
         <f>ROUND(income!$C$5 * $M44, 0)</f>
-        <v>24</v>
-      </c>
-      <c r="P44" s="7">
-        <f>ROUND(income!$D$5 * $M44, 0)</f>
-        <v>185</v>
+        <v>0</v>
       </c>
       <c r="Q44" s="7">
         <v>0</v>
@@ -9895,15 +9757,15 @@
       </c>
       <c r="N45" s="7">
         <f>ROUND(income!$B$5 * $M45, 0)</f>
-        <v>662</v>
+        <v>0</v>
       </c>
       <c r="O45" s="7">
+        <f>ROUND(income!$F$5 * $M45, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P45" s="7">
         <f>ROUND(income!$C$5 * $M45, 0)</f>
-        <v>24</v>
-      </c>
-      <c r="P45" s="7">
-        <f>ROUND(income!$D$5 * $M45, 0)</f>
-        <v>187</v>
+        <v>0</v>
       </c>
       <c r="Q45" s="7">
         <v>0</v>

</xml_diff>

<commit_message>
playthrough 3 updates finished
</commit_message>
<xml_diff>
--- a/backend/emporium/data/StageData.xlsx
+++ b/backend/emporium/data/StageData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="828" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="828" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="8" r:id="rId1"/>
@@ -5461,7 +5461,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="R1" sqref="R1"/>
     </sheetView>
@@ -5600,11 +5600,11 @@
         <v>1</v>
       </c>
       <c r="B5" s="1">
-        <f t="shared" ref="B5:B14" si="1">B4+1</f>
+        <f t="shared" ref="B5:C14" si="1">B4+1</f>
         <v>3</v>
       </c>
       <c r="C5" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D5" s="1">
         <v>2</v>
@@ -5639,7 +5639,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>
@@ -5674,10 +5674,11 @@
         <v>5</v>
       </c>
       <c r="C7" s="1">
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="D7" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M7" s="1">
         <v>1</v>
@@ -5715,10 +5716,10 @@
         <v>1</v>
       </c>
       <c r="E8" s="1">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F8" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
@@ -5758,10 +5759,10 @@
         <v>1</v>
       </c>
       <c r="E9" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F9" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M9" s="1">
         <v>2</v>
@@ -5799,7 +5800,7 @@
         <v>2</v>
       </c>
       <c r="E10" s="1">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F10" s="1">
         <v>1</v>
@@ -5834,13 +5835,13 @@
         <v>9</v>
       </c>
       <c r="C11" s="1">
+        <v>17</v>
+      </c>
+      <c r="D11" s="1">
+        <v>2</v>
+      </c>
+      <c r="E11" s="1">
         <v>18</v>
-      </c>
-      <c r="D11" s="1">
-        <v>1</v>
-      </c>
-      <c r="E11" s="1">
-        <v>17</v>
       </c>
       <c r="F11" s="1">
         <v>2</v>
@@ -5889,10 +5890,10 @@
         <v>1</v>
       </c>
       <c r="G12" s="1">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H12" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M12" s="1">
         <v>3</v>
@@ -5924,16 +5925,16 @@
         <v>11</v>
       </c>
       <c r="C13" s="1">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D13" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E13" s="1">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F13" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G13" s="1">
         <v>18</v>
@@ -5973,19 +5974,19 @@
         <v>12</v>
       </c>
       <c r="C14" s="1">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D14" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E14" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F14" s="1">
         <v>2</v>
       </c>
       <c r="G14" s="1">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H14" s="1">
         <v>2</v>
@@ -6086,11 +6087,11 @@
         <v>2</v>
       </c>
       <c r="B18" s="1">
-        <f t="shared" ref="B18:B27" si="4">B17+1</f>
+        <f t="shared" ref="B18:C27" si="4">B17+1</f>
         <v>3</v>
       </c>
       <c r="C18" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D18" s="1">
         <v>5</v>
@@ -6125,7 +6126,7 @@
         <v>4</v>
       </c>
       <c r="C19" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D19" s="1">
         <v>4</v>
@@ -6160,10 +6161,11 @@
         <v>5</v>
       </c>
       <c r="C20" s="1">
+        <f t="shared" si="4"/>
         <v>17</v>
       </c>
       <c r="D20" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M20" s="1">
         <v>1</v>
@@ -6201,10 +6203,10 @@
         <v>4</v>
       </c>
       <c r="E21" s="1">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F21" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
@@ -6244,10 +6246,10 @@
         <v>4</v>
       </c>
       <c r="E22" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F22" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M22" s="1">
         <v>2</v>
@@ -6285,7 +6287,7 @@
         <v>5</v>
       </c>
       <c r="E23" s="1">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F23" s="1">
         <v>4</v>
@@ -6320,13 +6322,13 @@
         <v>9</v>
       </c>
       <c r="C24" s="1">
+        <v>17</v>
+      </c>
+      <c r="D24" s="1">
+        <v>5</v>
+      </c>
+      <c r="E24" s="1">
         <v>18</v>
-      </c>
-      <c r="D24" s="1">
-        <v>4</v>
-      </c>
-      <c r="E24" s="1">
-        <v>17</v>
       </c>
       <c r="F24" s="1">
         <v>5</v>
@@ -6375,10 +6377,10 @@
         <v>4</v>
       </c>
       <c r="G25" s="1">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H25" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M25" s="1">
         <v>3</v>
@@ -6410,16 +6412,16 @@
         <v>11</v>
       </c>
       <c r="C26" s="1">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D26" s="1">
+        <v>5</v>
+      </c>
+      <c r="E26" s="1">
+        <v>18</v>
+      </c>
+      <c r="F26" s="1">
         <v>4</v>
-      </c>
-      <c r="E26" s="1">
-        <v>15</v>
-      </c>
-      <c r="F26" s="1">
-        <v>5</v>
       </c>
       <c r="G26" s="1">
         <v>18</v>
@@ -6459,19 +6461,19 @@
         <v>12</v>
       </c>
       <c r="C27" s="1">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D27" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E27" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F27" s="1">
         <v>5</v>
       </c>
       <c r="G27" s="1">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H27" s="1">
         <v>5</v>
@@ -6572,11 +6574,11 @@
         <v>3</v>
       </c>
       <c r="B31" s="1">
-        <f t="shared" ref="B31:B40" si="7">B30+1</f>
+        <f t="shared" ref="B31:C40" si="7">B30+1</f>
         <v>3</v>
       </c>
       <c r="C31" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D31" s="1">
         <v>8</v>
@@ -6611,7 +6613,7 @@
         <v>4</v>
       </c>
       <c r="C32" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D32" s="1">
         <v>7</v>
@@ -6646,10 +6648,11 @@
         <v>5</v>
       </c>
       <c r="C33" s="1">
+        <f t="shared" si="7"/>
         <v>17</v>
       </c>
       <c r="D33" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M33" s="1">
         <v>1</v>
@@ -6687,10 +6690,10 @@
         <v>7</v>
       </c>
       <c r="E34" s="1">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F34" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G34" s="7"/>
       <c r="H34" s="7"/>
@@ -6730,10 +6733,10 @@
         <v>7</v>
       </c>
       <c r="E35" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F35" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M35" s="1">
         <v>2</v>
@@ -6771,7 +6774,7 @@
         <v>8</v>
       </c>
       <c r="E36" s="1">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F36" s="1">
         <v>7</v>
@@ -6806,13 +6809,13 @@
         <v>9</v>
       </c>
       <c r="C37" s="1">
+        <v>17</v>
+      </c>
+      <c r="D37" s="1">
+        <v>8</v>
+      </c>
+      <c r="E37" s="1">
         <v>18</v>
-      </c>
-      <c r="D37" s="1">
-        <v>7</v>
-      </c>
-      <c r="E37" s="1">
-        <v>17</v>
       </c>
       <c r="F37" s="1">
         <v>8</v>
@@ -6861,10 +6864,10 @@
         <v>7</v>
       </c>
       <c r="G38" s="1">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H38" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M38" s="1">
         <v>3</v>
@@ -6896,16 +6899,16 @@
         <v>11</v>
       </c>
       <c r="C39" s="1">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D39" s="1">
+        <v>8</v>
+      </c>
+      <c r="E39" s="1">
+        <v>18</v>
+      </c>
+      <c r="F39" s="1">
         <v>7</v>
-      </c>
-      <c r="E39" s="1">
-        <v>15</v>
-      </c>
-      <c r="F39" s="1">
-        <v>8</v>
       </c>
       <c r="G39" s="1">
         <v>18</v>
@@ -6945,19 +6948,19 @@
         <v>12</v>
       </c>
       <c r="C40" s="1">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D40" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E40" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F40" s="1">
         <v>8</v>
       </c>
       <c r="G40" s="1">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H40" s="1">
         <v>8</v>
@@ -7821,7 +7824,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="R1" sqref="R1"/>
     </sheetView>
@@ -7891,27 +7894,7 @@
       <c r="A3" s="9">
         <v>1</v>
       </c>
-      <c r="B3" s="9">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1">
-        <v>13</v>
-      </c>
-      <c r="D3" s="1">
-        <v>1</v>
-      </c>
-      <c r="E3" s="1">
-        <v>14</v>
-      </c>
-      <c r="F3" s="1">
-        <v>1</v>
-      </c>
-      <c r="G3" s="1">
-        <v>13</v>
-      </c>
-      <c r="H3" s="1">
-        <v>2</v>
-      </c>
+      <c r="B3" s="9"/>
       <c r="M3" s="1">
         <v>3</v>
       </c>
@@ -7958,7 +7941,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="1">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D5" s="1">
         <v>4</v>
@@ -7967,13 +7950,13 @@
         <v>14</v>
       </c>
       <c r="F5" s="1">
+        <v>4</v>
+      </c>
+      <c r="G5" s="1">
+        <v>13</v>
+      </c>
+      <c r="H5" s="1">
         <v>5</v>
-      </c>
-      <c r="G5" s="1">
-        <v>17</v>
-      </c>
-      <c r="H5" s="1">
-        <v>4</v>
       </c>
       <c r="M5" s="1">
         <v>3</v>
@@ -8021,22 +8004,22 @@
         <v>1</v>
       </c>
       <c r="C7" s="1">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D7" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E7" s="1">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F7" s="1">
         <v>7</v>
       </c>
       <c r="G7" s="1">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H7" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -8084,33 +8067,15 @@
       <c r="A9" s="10">
         <v>4</v>
       </c>
-      <c r="B9" s="10">
-        <v>1</v>
-      </c>
-      <c r="C9" s="7">
-        <v>13</v>
-      </c>
-      <c r="D9" s="7">
-        <v>2</v>
-      </c>
-      <c r="E9" s="7">
-        <v>16</v>
-      </c>
-      <c r="F9" s="7">
-        <v>1</v>
-      </c>
-      <c r="G9" s="7">
-        <v>17</v>
-      </c>
-      <c r="H9" s="7">
-        <v>1</v>
-      </c>
-      <c r="I9" s="7">
-        <v>17</v>
-      </c>
-      <c r="J9" s="7">
-        <v>2</v>
-      </c>
+      <c r="B9" s="10"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1">
@@ -8155,33 +8120,15 @@
       <c r="A11" s="10">
         <v>5</v>
       </c>
-      <c r="B11" s="10">
-        <v>1</v>
-      </c>
-      <c r="C11" s="1">
-        <v>16</v>
-      </c>
-      <c r="D11" s="1">
-        <v>1</v>
-      </c>
-      <c r="E11" s="1">
-        <v>15</v>
-      </c>
-      <c r="F11" s="1">
-        <v>2</v>
-      </c>
-      <c r="G11" s="1">
-        <v>16</v>
-      </c>
-      <c r="H11" s="1">
-        <v>2</v>
-      </c>
-      <c r="I11" s="1">
-        <v>19</v>
-      </c>
-      <c r="J11" s="1">
-        <v>1</v>
-      </c>
+      <c r="B11" s="10"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1">
@@ -8226,33 +8173,15 @@
       <c r="A13" s="10">
         <v>6</v>
       </c>
-      <c r="B13" s="10">
-        <v>1</v>
-      </c>
-      <c r="C13" s="1">
-        <v>14</v>
-      </c>
-      <c r="D13" s="1">
-        <v>2</v>
-      </c>
-      <c r="E13" s="1">
-        <v>17</v>
-      </c>
-      <c r="F13" s="1">
-        <v>1</v>
-      </c>
-      <c r="G13" s="1">
-        <v>19</v>
-      </c>
-      <c r="H13" s="1">
-        <v>1</v>
-      </c>
-      <c r="I13" s="1">
-        <v>18</v>
-      </c>
-      <c r="J13" s="1">
-        <v>2</v>
-      </c>
+      <c r="B13" s="10"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1">

</xml_diff>

<commit_message>
heists converted to using dynamic difficulty
</commit_message>
<xml_diff>
--- a/backend/emporium/data/StageData.xlsx
+++ b/backend/emporium/data/StageData.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="129">
   <si>
     <t>Name</t>
   </si>
@@ -386,6 +386,36 @@
   </si>
   <si>
     <t>6 hr</t>
+  </si>
+  <si>
+    <t>DifficultyL1</t>
+  </si>
+  <si>
+    <t>DifficultyL2</t>
+  </si>
+  <si>
+    <t>DifficultyL3</t>
+  </si>
+  <si>
+    <t>DifficultyL4</t>
+  </si>
+  <si>
+    <t>DifficultyL5</t>
+  </si>
+  <si>
+    <t>easy</t>
+  </si>
+  <si>
+    <t>easy / med</t>
+  </si>
+  <si>
+    <t>med</t>
+  </si>
+  <si>
+    <t>hard</t>
+  </si>
+  <si>
+    <t>med / hard</t>
   </si>
 </sst>
 </file>
@@ -395,7 +425,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -407,6 +437,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -438,7 +475,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -496,6 +533,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7244,8 +7284,8 @@
         <v>46</v>
       </c>
       <c r="Q6" s="7">
-        <f>ROUND(constants!D$3 / 2 * $N6, 0)</f>
-        <v>5</v>
+        <f>ROUND(constants!D$4 / 2 * $N6, 0)</f>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.3">
@@ -7285,8 +7325,8 @@
         <v>51</v>
       </c>
       <c r="Q7" s="7">
-        <f>ROUND(constants!D$3 / 2 * $N7, 0)</f>
-        <v>6</v>
+        <f>ROUND(constants!D$4 / 2 * $N7, 0)</f>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.3">
@@ -7344,8 +7384,8 @@
         <v>53</v>
       </c>
       <c r="Q9" s="7">
-        <f>ROUND(constants!D$3 / 2 * $N9, 0)</f>
-        <v>6</v>
+        <f>ROUND(constants!D$5 / 2 * $N9, 0)</f>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.3">
@@ -7385,8 +7425,8 @@
         <v>58</v>
       </c>
       <c r="Q10" s="7">
-        <f>ROUND(constants!D$3 / 2 * $N10, 0)</f>
-        <v>6</v>
+        <f>ROUND(constants!D$5 / 2 * $N10, 0)</f>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.3">
@@ -7444,8 +7484,8 @@
         <v>60</v>
       </c>
       <c r="Q12" s="7">
-        <f>ROUND(constants!D$3 / 2 * $N12, 0)</f>
-        <v>6</v>
+        <f>ROUND(constants!D$6 / 2 * $N12, 0)</f>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.3">
@@ -7489,8 +7529,8 @@
         <v>130</v>
       </c>
       <c r="Q13" s="7">
-        <f>ROUND(constants!D$3 / 2 * $N13, 0)</f>
-        <v>6</v>
+        <f>ROUND(constants!D$6 / 2 * $N13, 0)</f>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.3">
@@ -7548,8 +7588,8 @@
         <v>67</v>
       </c>
       <c r="Q15" s="7">
-        <f>ROUND(constants!D$3 / 2 * $N15, 0)</f>
-        <v>6</v>
+        <f>ROUND(constants!D$7 / 2 * $N15, 0)</f>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.3">
@@ -7593,8 +7633,8 @@
         <v>146</v>
       </c>
       <c r="Q16" s="7">
-        <f>ROUND(constants!D$3 / 2 * $N16, 0)</f>
-        <v>7</v>
+        <f>ROUND(constants!D$7 / 2 * $N16, 0)</f>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -7647,8 +7687,8 @@
         <v>150</v>
       </c>
       <c r="Q18" s="7">
-        <f>ROUND(constants!D$3 / 2 * $N18, 0)</f>
-        <v>6</v>
+        <f>ROUND(constants!D$8 / 2 * $N18, 0)</f>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -7692,8 +7732,8 @@
         <v>162</v>
       </c>
       <c r="Q19" s="7">
-        <f>ROUND(constants!D$3 / 2 * $N19, 0)</f>
-        <v>7</v>
+        <f>ROUND(constants!D$8 / 2 * $N19, 0)</f>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -7904,22 +7944,22 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S23"/>
+  <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R1" sqref="R1"/>
+      <selection pane="bottomLeft" activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="8.77734375" style="1" customWidth="1"/>
-    <col min="3" max="13" width="10.77734375" style="1" customWidth="1"/>
-    <col min="14" max="17" width="8.77734375" style="1" customWidth="1"/>
-    <col min="18" max="18" width="1.77734375" customWidth="1"/>
+    <col min="3" max="8" width="10.77734375" style="1" customWidth="1"/>
+    <col min="9" max="12" width="8.77734375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="1.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>10</v>
       </c>
@@ -7927,76 +7967,61 @@
         <v>38</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>101</v>
+        <v>119</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>102</v>
+        <v>121</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>104</v>
+        <v>47</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>108</v>
+        <v>39</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>105</v>
+        <v>41</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q1" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="9">
         <v>1</v>
       </c>
       <c r="B3" s="9"/>
-      <c r="M3" s="1">
-        <v>3</v>
-      </c>
-      <c r="N3" s="15">
-        <v>3</v>
-      </c>
-      <c r="O3" s="7">
-        <f>ROUND(constants!B$3 *$M3 * $N3, 0)</f>
+      <c r="H3" s="1">
+        <v>3</v>
+      </c>
+      <c r="I3" s="15">
+        <v>3</v>
+      </c>
+      <c r="J3" s="7">
+        <f>ROUND(constants!B$3 *$H3 * $I3, 0)</f>
         <v>450</v>
       </c>
-      <c r="P3" s="7">
-        <f>ROUND(constants!C$3 *$M3 * $N3, 0)</f>
+      <c r="K3" s="7">
+        <f>ROUND(constants!C$3 *$H3 * $I3, 0)</f>
         <v>180</v>
       </c>
-      <c r="Q3" s="7">
-        <f>ROUND(constants!D$3 / 3 * $N3, 0)</f>
+      <c r="L3" s="7">
+        <f>ROUND(constants!D$3 / 3 * $I3, 0)</f>
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="9"/>
       <c r="B4" s="9"/>
       <c r="C4" s="7"/>
@@ -8005,61 +8030,47 @@
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
+      <c r="I4" s="15"/>
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
       <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="15"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="7"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="9">
         <v>2</v>
       </c>
       <c r="B5" s="9">
         <v>1</v>
       </c>
-      <c r="C5" s="1">
-        <v>13</v>
-      </c>
-      <c r="D5" s="1">
-        <v>4</v>
-      </c>
-      <c r="E5" s="1">
-        <v>14</v>
-      </c>
-      <c r="F5" s="1">
-        <v>4</v>
-      </c>
-      <c r="G5" s="1">
-        <v>13</v>
+      <c r="C5" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>126</v>
       </c>
       <c r="H5" s="1">
-        <v>5</v>
-      </c>
-      <c r="M5" s="1">
-        <v>3</v>
-      </c>
-      <c r="N5" s="15">
+        <v>3</v>
+      </c>
+      <c r="I5" s="15">
         <v>3.1</v>
       </c>
-      <c r="O5" s="7">
-        <f>ROUND(constants!B$4 *$M5 * $N5, 0)</f>
+      <c r="J5" s="7">
+        <f>ROUND(constants!B$4 *$H5 * $I5, 0)</f>
         <v>493</v>
       </c>
-      <c r="P5" s="7">
-        <f>ROUND(constants!C$4 *$M5 * $N5, 0)</f>
+      <c r="K5" s="7">
+        <f>ROUND(constants!C$4 *$H5 * $I5, 0)</f>
         <v>205</v>
       </c>
-      <c r="Q5" s="7">
-        <f>ROUND(constants!D$3 / 3 * $N5, 0)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L5" s="7">
+        <f>ROUND(constants!D$4 / 3 * $I5, 0)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10"/>
       <c r="B6" s="10"/>
       <c r="C6" s="7"/>
@@ -8068,65 +8079,49 @@
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
+      <c r="I6" s="15"/>
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="15"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="7"/>
-    </row>
-    <row r="7" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10">
         <v>3</v>
       </c>
       <c r="B7" s="10">
         <v>1</v>
       </c>
-      <c r="C7" s="1">
-        <v>12</v>
-      </c>
-      <c r="D7" s="1">
+      <c r="C7" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1">
+        <v>3</v>
+      </c>
+      <c r="I7" s="15">
+        <v>3.2</v>
+      </c>
+      <c r="J7" s="7">
+        <f>ROUND(constants!B$5 *$H7 * $I7, 0)</f>
+        <v>538</v>
+      </c>
+      <c r="K7" s="7">
+        <f>ROUND(constants!C$5 *$H7 * $I7, 0)</f>
+        <v>230</v>
+      </c>
+      <c r="L7" s="7">
+        <f>ROUND(constants!D$5 / 3 * $I7, 0)</f>
         <v>7</v>
       </c>
-      <c r="E7" s="1">
-        <v>15</v>
-      </c>
-      <c r="F7" s="1">
-        <v>7</v>
-      </c>
-      <c r="G7" s="1">
-        <v>15</v>
-      </c>
-      <c r="H7" s="1">
-        <v>8</v>
-      </c>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1">
-        <v>3</v>
-      </c>
-      <c r="N7" s="15">
-        <v>3.2</v>
-      </c>
-      <c r="O7" s="7">
-        <f>ROUND(constants!B$5 *$M7 * $N7, 0)</f>
-        <v>538</v>
-      </c>
-      <c r="P7" s="7">
-        <f>ROUND(constants!C$5 *$M7 * $N7, 0)</f>
-        <v>230</v>
-      </c>
-      <c r="Q7" s="7">
-        <f>ROUND(constants!D$3 / 3 * $N7, 0)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10"/>
       <c r="B8" s="10"/>
       <c r="C8" s="7"/>
@@ -8135,51 +8130,51 @@
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
+      <c r="I8" s="15"/>
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
       <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="15"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="7"/>
-    </row>
-    <row r="9" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10">
         <v>4</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
+      <c r="B9" s="10">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>126</v>
+      </c>
       <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1">
+      <c r="H9" s="1">
         <v>4</v>
       </c>
-      <c r="N9" s="15">
+      <c r="I9" s="15">
         <v>3.3</v>
       </c>
-      <c r="O9" s="7">
-        <f>ROUND(constants!B$6 *$M9 * $N9, 0)</f>
+      <c r="J9" s="7">
+        <f>ROUND(constants!B$6 *$H9 * $I9, 0)</f>
         <v>779</v>
       </c>
-      <c r="P9" s="7">
-        <f>ROUND(constants!C$6 *$M9 * $N9, 0)</f>
+      <c r="K9" s="7">
+        <f>ROUND(constants!C$6 *$H9 * $I9, 0)</f>
         <v>343</v>
       </c>
-      <c r="Q9" s="7">
-        <f>ROUND(constants!D$3 / 3 * $N9, 0)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L9" s="7">
+        <f>ROUND(constants!D$6 / 3 * $I9, 0)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10"/>
       <c r="B10" s="10"/>
       <c r="C10" s="7"/>
@@ -8188,51 +8183,51 @@
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
+      <c r="I10" s="15"/>
       <c r="J10" s="7"/>
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="15"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="7"/>
-      <c r="Q10" s="7"/>
-    </row>
-    <row r="11" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10">
         <v>5</v>
       </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
+      <c r="B11" s="10">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>126</v>
+      </c>
       <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1">
+      <c r="H11" s="1">
         <v>4</v>
       </c>
-      <c r="N11" s="15">
+      <c r="I11" s="15">
         <v>3.4</v>
       </c>
-      <c r="O11" s="7">
-        <f>ROUND(constants!B$7 *$M11 * $N11, 0)</f>
+      <c r="J11" s="7">
+        <f>ROUND(constants!B$7 *$H11 * $I11, 0)</f>
         <v>843</v>
       </c>
-      <c r="P11" s="7">
-        <f>ROUND(constants!C$7 *$M11 * $N11, 0)</f>
+      <c r="K11" s="7">
+        <f>ROUND(constants!C$7 *$H11 * $I11, 0)</f>
         <v>381</v>
       </c>
-      <c r="Q11" s="7">
-        <f>ROUND(constants!D$3 / 3 * $N11, 0)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L11" s="7">
+        <f>ROUND(constants!D$7 / 3 * $I11, 0)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10"/>
       <c r="B12" s="10"/>
       <c r="C12" s="7"/>
@@ -8241,59 +8236,59 @@
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
+      <c r="I12" s="15"/>
       <c r="J12" s="7"/>
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="15"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="7"/>
-      <c r="Q12" s="7"/>
-    </row>
-    <row r="13" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10">
         <v>6</v>
       </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
+      <c r="B13" s="10">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>126</v>
+      </c>
       <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1">
+      <c r="H13" s="1">
         <v>4</v>
       </c>
-      <c r="N13" s="15">
+      <c r="I13" s="15">
         <v>3.5</v>
       </c>
-      <c r="O13" s="7">
-        <f>ROUND(constants!B$8 *$M13 * $N13, 0)</f>
+      <c r="J13" s="7">
+        <f>ROUND(constants!B$8 *$H13 * $I13, 0)</f>
         <v>910</v>
       </c>
-      <c r="P13" s="7">
-        <f>ROUND(constants!C$8 *$M13 * $N13, 0)</f>
+      <c r="K13" s="7">
+        <f>ROUND(constants!C$8 *$H13 * $I13, 0)</f>
         <v>420</v>
       </c>
-      <c r="Q13" s="7">
-        <f>ROUND(constants!D$3 / 3 * $N13, 0)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L13" s="7">
+        <f>ROUND(constants!D$8 / 3 * $I13, 0)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10"/>
       <c r="B14" s="10"/>
-      <c r="N14" s="15"/>
-      <c r="O14" s="7"/>
-      <c r="P14" s="7"/>
-      <c r="Q14" s="7"/>
-    </row>
-    <row r="15" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="I14" s="15"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+    </row>
+    <row r="15" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10">
         <v>7</v>
       </c>
@@ -8303,37 +8298,34 @@
       <c r="E15" s="14"/>
       <c r="F15" s="14"/>
       <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14">
+      <c r="H15" s="14">
         <v>5</v>
       </c>
-      <c r="N15" s="15">
+      <c r="I15" s="15">
         <v>3.6</v>
       </c>
-      <c r="O15" s="7">
-        <f>ROUND(constants!B$9 *$M15 * $N15, 0)</f>
+      <c r="J15" s="7">
+        <f>ROUND(constants!B$9 *$H15 * $I15, 0)</f>
         <v>1224</v>
       </c>
-      <c r="P15" s="7">
-        <f>ROUND(constants!C$9 *$M15 * $N15, 0)</f>
+      <c r="K15" s="7">
+        <f>ROUND(constants!C$9 *$H15 * $I15, 0)</f>
         <v>576</v>
       </c>
-      <c r="Q15" s="7">
-        <f>ROUND(constants!D$3 / 3 * $N15, 0)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L15" s="7">
+        <f>ROUND(constants!D$9 / 3 * $I15, 0)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10"/>
       <c r="B16" s="10"/>
-      <c r="N16" s="15"/>
-      <c r="O16" s="7"/>
-      <c r="P16" s="7"/>
-      <c r="Q16" s="7"/>
-    </row>
-    <row r="17" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="I16" s="15"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+    </row>
+    <row r="17" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10">
         <v>8</v>
       </c>
@@ -8343,39 +8335,34 @@
       <c r="E17" s="14"/>
       <c r="F17" s="14"/>
       <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="14">
+      <c r="H17" s="14">
         <v>5</v>
       </c>
-      <c r="N17" s="15">
+      <c r="I17" s="15">
         <v>3.7</v>
       </c>
-      <c r="O17" s="7">
-        <f>ROUND(constants!B$10 *$M17 * $N17, 0)</f>
+      <c r="J17" s="7">
+        <f>ROUND(constants!B$10 *$H17 * $I17, 0)</f>
         <v>1314</v>
       </c>
-      <c r="P17" s="7">
-        <f>ROUND(constants!C$10 *$M17 * $N17, 0)</f>
+      <c r="K17" s="7">
+        <f>ROUND(constants!C$10 *$H17 * $I17, 0)</f>
         <v>629</v>
       </c>
-      <c r="Q17" s="7">
-        <f>ROUND(constants!D$3 / 3 * $N17, 0)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L17" s="7">
+        <f>ROUND(constants!D$10 / 3 * $I17, 0)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10"/>
       <c r="B18" s="10"/>
-      <c r="N18" s="15"/>
-      <c r="O18" s="7"/>
-      <c r="P18" s="7"/>
-      <c r="Q18" s="7"/>
-    </row>
-    <row r="19" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="I18" s="15"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+    </row>
+    <row r="19" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="10">
         <v>9</v>
       </c>
@@ -8385,31 +8372,26 @@
       <c r="E19" s="14"/>
       <c r="F19" s="14"/>
       <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
-      <c r="M19" s="14">
+      <c r="H19" s="14">
         <v>5</v>
       </c>
-      <c r="N19" s="15">
+      <c r="I19" s="15">
         <v>3.8</v>
       </c>
-      <c r="O19" s="7">
-        <f>ROUND(constants!B$11 *$M19 * $N19, 0)</f>
+      <c r="J19" s="7">
+        <f>ROUND(constants!B$11 *$H19 * $I19, 0)</f>
         <v>1406</v>
       </c>
-      <c r="P19" s="7">
-        <f>ROUND(constants!C$11 *$M19 * $N19, 0)</f>
+      <c r="K19" s="7">
+        <f>ROUND(constants!C$11 *$H19 * $I19, 0)</f>
         <v>684</v>
       </c>
-      <c r="Q19" s="7">
-        <f>ROUND(constants!D$3 / 3 * $N19, 0)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L19" s="7">
+        <f>ROUND(constants!D$11 / 3 * $I19, 0)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="10"/>
       <c r="B20" s="10"/>
       <c r="C20" s="11"/>
@@ -8418,19 +8400,14 @@
       <c r="F20" s="11"/>
       <c r="G20" s="11"/>
       <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
+      <c r="I20" s="15"/>
       <c r="J20" s="11"/>
       <c r="K20" s="11"/>
       <c r="L20" s="11"/>
       <c r="M20" s="11"/>
-      <c r="N20" s="15"/>
-      <c r="O20" s="11"/>
-      <c r="P20" s="11"/>
-      <c r="Q20" s="11"/>
-      <c r="R20" s="11"/>
-      <c r="S20" s="11"/>
-    </row>
-    <row r="21" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N20" s="11"/>
+    </row>
+    <row r="21" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C21" s="14"/>
       <c r="D21" s="14"/>
       <c r="E21" s="14"/>
@@ -8439,16 +8416,11 @@
       <c r="H21" s="14"/>
       <c r="I21" s="14"/>
       <c r="J21" s="14"/>
-      <c r="K21" s="14"/>
       <c r="L21" s="14"/>
-      <c r="M21" s="14"/>
-      <c r="N21" s="14"/>
-      <c r="O21" s="14"/>
-      <c r="Q21" s="14"/>
-      <c r="R21" s="13"/>
-      <c r="S21" s="13"/>
-    </row>
-    <row r="22" spans="1:19" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M21" s="13"/>
+      <c r="N21" s="13"/>
+    </row>
+    <row r="22" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="12"/>
       <c r="B22" s="12"/>
       <c r="C22" s="12"/>
@@ -8461,13 +8433,8 @@
       <c r="J22" s="12"/>
       <c r="K22" s="12"/>
       <c r="L22" s="12"/>
-      <c r="M22" s="12"/>
-      <c r="N22" s="12"/>
-      <c r="O22" s="12"/>
-      <c r="P22" s="12"/>
-      <c r="Q22" s="12"/>
-    </row>
-    <row r="23" spans="1:19" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="12"/>
       <c r="B23" s="12"/>
       <c r="C23" s="12"/>
@@ -8480,11 +8447,6 @@
       <c r="J23" s="12"/>
       <c r="K23" s="12"/>
       <c r="L23" s="12"/>
-      <c r="M23" s="12"/>
-      <c r="N23" s="12"/>
-      <c r="O23" s="12"/>
-      <c r="P23" s="12"/>
-      <c r="Q23" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8494,22 +8456,22 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q45"/>
+  <dimension ref="A1:L45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R1" sqref="R1"/>
+      <selection pane="bottomLeft" activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="8.77734375" style="1" customWidth="1"/>
-    <col min="3" max="13" width="10.77734375" style="1" customWidth="1"/>
-    <col min="14" max="17" width="8.77734375" style="1" customWidth="1"/>
-    <col min="18" max="18" width="1.77734375" customWidth="1"/>
+    <col min="3" max="8" width="10.77734375" style="1" customWidth="1"/>
+    <col min="9" max="12" width="8.77734375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="1.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>10</v>
       </c>
@@ -8517,84 +8479,66 @@
         <v>38</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>101</v>
+        <v>119</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>102</v>
+        <v>121</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>104</v>
+        <v>47</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>108</v>
+        <v>39</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>105</v>
+        <v>41</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q1" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="9">
         <v>1</v>
       </c>
       <c r="B3" s="9">
         <v>1</v>
       </c>
-      <c r="C3" s="1">
-        <v>13</v>
-      </c>
-      <c r="D3" s="1">
-        <v>1</v>
-      </c>
-      <c r="M3" s="1">
-        <v>1</v>
-      </c>
-      <c r="N3" s="16">
+      <c r="C3" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1</v>
+      </c>
+      <c r="I3" s="16">
         <v>4</v>
       </c>
-      <c r="O3" s="7">
-        <f>ROUND(constants!B$3 * $M3 * $N3,0)</f>
+      <c r="J3" s="7">
+        <f>ROUND(constants!B$3 * $H3 * $I3,0)</f>
         <v>200</v>
       </c>
-      <c r="P3" s="7">
-        <f>ROUND(constants!C$3 * $M3 * $N3,0)</f>
+      <c r="K3" s="7">
+        <f>ROUND(constants!C$3 * $H3 * $I3,0)</f>
         <v>80</v>
       </c>
-      <c r="Q3" s="7">
-        <f>ROUND(constants!D$3 /4 * $N3,0)</f>
+      <c r="L3" s="7">
+        <f>ROUND(constants!D$3 /4 * $I3,0)</f>
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <f>A3</f>
         <v>1</v>
@@ -8603,33 +8547,30 @@
         <f>B3+1</f>
         <v>2</v>
       </c>
-      <c r="C4" s="1">
-        <v>12</v>
-      </c>
-      <c r="D4" s="1">
-        <v>2</v>
-      </c>
-      <c r="M4" s="1">
-        <v>1</v>
-      </c>
-      <c r="N4" s="16">
-        <f>N3+0.05</f>
+      <c r="C4" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1</v>
+      </c>
+      <c r="I4" s="16">
+        <f>I3+0.05</f>
         <v>4.05</v>
       </c>
-      <c r="O4" s="7">
-        <f>ROUND(constants!B$3 * $M4 * $N4,0)</f>
+      <c r="J4" s="7">
+        <f>ROUND(constants!B$3 * $H4 * $I4,0)</f>
         <v>203</v>
       </c>
-      <c r="P4" s="7">
-        <f>ROUND(constants!C$3 * $M4 * $N4,0)</f>
+      <c r="K4" s="7">
+        <f>ROUND(constants!C$3 * $H4 * $I4,0)</f>
         <v>81</v>
       </c>
-      <c r="Q4" s="7">
-        <f>ROUND(constants!D$3 /4 * $N4,0)</f>
+      <c r="L4" s="7">
+        <f>ROUND(constants!D$3 /4 * $I4,0)</f>
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="9">
         <f t="shared" ref="A5:A12" si="0">A4</f>
         <v>1</v>
@@ -8638,33 +8579,33 @@
         <f t="shared" ref="B5:B12" si="1">B4+1</f>
         <v>3</v>
       </c>
-      <c r="C5" s="1">
-        <v>15</v>
-      </c>
-      <c r="D5" s="1">
-        <v>1</v>
-      </c>
-      <c r="M5" s="1">
-        <v>1</v>
-      </c>
-      <c r="N5" s="16">
-        <f t="shared" ref="N5:N12" si="2">N4+0.05</f>
+      <c r="C5" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H5" s="1">
+        <v>2</v>
+      </c>
+      <c r="I5" s="16">
+        <f t="shared" ref="I5:I12" si="2">I4+0.05</f>
         <v>4.0999999999999996</v>
       </c>
-      <c r="O5" s="7">
-        <f>ROUND(constants!B$3 * $M5 * $N5,0)</f>
-        <v>205</v>
-      </c>
-      <c r="P5" s="7">
-        <f>ROUND(constants!C$3 * $M5 * $N5,0)</f>
-        <v>82</v>
-      </c>
-      <c r="Q5" s="7">
-        <f>ROUND(constants!D$3 /4 * $N5,0)</f>
+      <c r="J5" s="7">
+        <f>ROUND(constants!B$3 * $H5 * $I5,0)</f>
+        <v>410</v>
+      </c>
+      <c r="K5" s="7">
+        <f>ROUND(constants!C$3 * $H5 * $I5,0)</f>
+        <v>164</v>
+      </c>
+      <c r="L5" s="7">
+        <f>ROUND(constants!D$3 /4 * $I5,0)</f>
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="9">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -8673,39 +8614,33 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="C6" s="1">
-        <v>12</v>
-      </c>
-      <c r="D6" s="1">
-        <v>1</v>
-      </c>
-      <c r="E6" s="1">
-        <v>13</v>
-      </c>
-      <c r="F6" s="1">
-        <v>1</v>
-      </c>
-      <c r="M6" s="1">
-        <v>2</v>
-      </c>
-      <c r="N6" s="16">
+      <c r="C6" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H6" s="1">
+        <v>2</v>
+      </c>
+      <c r="I6" s="16">
         <f t="shared" si="2"/>
         <v>4.1499999999999995</v>
       </c>
-      <c r="O6" s="7">
-        <f>ROUND(constants!B$3 * $M6 * $N6,0)</f>
+      <c r="J6" s="7">
+        <f>ROUND(constants!B$3 * $H6 * $I6,0)</f>
         <v>415</v>
       </c>
-      <c r="P6" s="7">
-        <f>ROUND(constants!C$3 * $M6 * $N6,0)</f>
+      <c r="K6" s="7">
+        <f>ROUND(constants!C$3 * $H6 * $I6,0)</f>
         <v>166</v>
       </c>
-      <c r="Q6" s="7">
-        <f>ROUND(constants!D$3 /4 * $N6,0)</f>
+      <c r="L6" s="7">
+        <f>ROUND(constants!D$3 /4 * $I6,0)</f>
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -8714,33 +8649,30 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="C7" s="1">
-        <v>14</v>
-      </c>
-      <c r="D7" s="1">
-        <v>1</v>
-      </c>
-      <c r="M7" s="1">
-        <v>1</v>
-      </c>
-      <c r="N7" s="16">
+      <c r="C7" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H7" s="1">
+        <v>1</v>
+      </c>
+      <c r="I7" s="16">
         <f t="shared" si="2"/>
         <v>4.1999999999999993</v>
       </c>
-      <c r="O7" s="7">
-        <f>ROUND(constants!B$3 * $M7 * $N7,0)</f>
+      <c r="J7" s="7">
+        <f>ROUND(constants!B$3 * $H7 * $I7,0)</f>
         <v>210</v>
       </c>
-      <c r="P7" s="7">
-        <f>ROUND(constants!C$3 * $M7 * $N7,0)</f>
+      <c r="K7" s="7">
+        <f>ROUND(constants!C$3 * $H7 * $I7,0)</f>
         <v>84</v>
       </c>
-      <c r="Q7" s="7">
-        <f>ROUND(constants!D$3 /4 * $N7,0)</f>
+      <c r="L7" s="7">
+        <f>ROUND(constants!D$3 /4 * $I7,0)</f>
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -8749,41 +8681,34 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="C8" s="1">
-        <v>14</v>
-      </c>
-      <c r="D8" s="1">
-        <v>1</v>
-      </c>
-      <c r="E8" s="1">
-        <v>13</v>
-      </c>
-      <c r="F8" s="1">
-        <v>2</v>
+      <c r="C8" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>126</v>
       </c>
       <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="M8" s="1">
-        <v>2</v>
-      </c>
-      <c r="N8" s="16">
+      <c r="H8" s="1">
+        <v>2</v>
+      </c>
+      <c r="I8" s="16">
         <f t="shared" si="2"/>
         <v>4.2499999999999991</v>
       </c>
-      <c r="O8" s="7">
-        <f>ROUND(constants!B$3 * $M8 * $N8,0)</f>
+      <c r="J8" s="7">
+        <f>ROUND(constants!B$3 * $H8 * $I8,0)</f>
         <v>425</v>
       </c>
-      <c r="P8" s="7">
-        <f>ROUND(constants!C$3 * $M8 * $N8,0)</f>
+      <c r="K8" s="7">
+        <f>ROUND(constants!C$3 * $H8 * $I8,0)</f>
         <v>170</v>
       </c>
-      <c r="Q8" s="7">
-        <f>ROUND(constants!D$3 /4 * $N8,0)</f>
+      <c r="L8" s="7">
+        <f>ROUND(constants!D$3 /4 * $I8,0)</f>
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -8792,33 +8717,30 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="C9" s="1">
-        <v>12</v>
-      </c>
-      <c r="D9" s="1">
-        <v>2</v>
-      </c>
-      <c r="M9" s="1">
-        <v>1</v>
-      </c>
-      <c r="N9" s="16">
+      <c r="C9" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H9" s="1">
+        <v>1</v>
+      </c>
+      <c r="I9" s="16">
         <f t="shared" si="2"/>
         <v>4.2999999999999989</v>
       </c>
-      <c r="O9" s="7">
-        <f>ROUND(constants!B$3 * $M9 * $N9,0)</f>
+      <c r="J9" s="7">
+        <f>ROUND(constants!B$3 * $H9 * $I9,0)</f>
         <v>215</v>
       </c>
-      <c r="P9" s="7">
-        <f>ROUND(constants!C$3 * $M9 * $N9,0)</f>
+      <c r="K9" s="7">
+        <f>ROUND(constants!C$3 * $H9 * $I9,0)</f>
         <v>86</v>
       </c>
-      <c r="Q9" s="7">
-        <f>ROUND(constants!D$3 /4 * $N9,0)</f>
+      <c r="L9" s="7">
+        <f>ROUND(constants!D$3 /4 * $I9,0)</f>
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -8827,45 +8749,36 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="C10" s="1">
-        <v>12</v>
-      </c>
-      <c r="D10" s="1">
-        <v>1</v>
-      </c>
-      <c r="E10" s="1">
-        <v>14</v>
-      </c>
-      <c r="F10" s="1">
-        <v>1</v>
-      </c>
-      <c r="G10" s="1">
-        <v>12</v>
+      <c r="C10" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>126</v>
       </c>
       <c r="H10" s="1">
-        <v>2</v>
-      </c>
-      <c r="M10" s="1">
-        <v>3</v>
-      </c>
-      <c r="N10" s="16">
+        <v>3</v>
+      </c>
+      <c r="I10" s="16">
         <f t="shared" si="2"/>
         <v>4.3499999999999988</v>
       </c>
-      <c r="O10" s="7">
-        <f>ROUND(constants!B$3 * $M10 * $N10,0)</f>
+      <c r="J10" s="7">
+        <f>ROUND(constants!B$3 * $H10 * $I10,0)</f>
         <v>653</v>
       </c>
-      <c r="P10" s="7">
-        <f>ROUND(constants!C$3 * $M10 * $N10,0)</f>
+      <c r="K10" s="7">
+        <f>ROUND(constants!C$3 * $H10 * $I10,0)</f>
         <v>261</v>
       </c>
-      <c r="Q10" s="7">
-        <f>ROUND(constants!D$3 /4 * $N10,0)</f>
+      <c r="L10" s="7">
+        <f>ROUND(constants!D$3 /4 * $I10,0)</f>
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="9">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -8874,39 +8787,33 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="C11" s="1">
-        <v>15</v>
-      </c>
-      <c r="D11" s="1">
-        <v>1</v>
-      </c>
-      <c r="E11" s="1">
-        <v>13</v>
-      </c>
-      <c r="F11" s="1">
-        <v>2</v>
-      </c>
-      <c r="M11" s="1">
-        <v>2</v>
-      </c>
-      <c r="N11" s="16">
+      <c r="C11" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="H11" s="1">
+        <v>2</v>
+      </c>
+      <c r="I11" s="16">
         <f t="shared" si="2"/>
         <v>4.3999999999999986</v>
       </c>
-      <c r="O11" s="7">
-        <f>ROUND(constants!B$3 * $M11 * $N11,0)</f>
+      <c r="J11" s="7">
+        <f>ROUND(constants!B$3 * $H11 * $I11,0)</f>
         <v>440</v>
       </c>
-      <c r="P11" s="7">
-        <f>ROUND(constants!C$3 * $M11 * $N11,0)</f>
+      <c r="K11" s="7">
+        <f>ROUND(constants!C$3 * $H11 * $I11,0)</f>
         <v>176</v>
       </c>
-      <c r="Q11" s="7">
-        <f>ROUND(constants!D$3 /4 * $N11,0)</f>
+      <c r="L11" s="7">
+        <f>ROUND(constants!D$3 /4 * $I11,0)</f>
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="9">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -8915,94 +8822,77 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="C12" s="1">
-        <v>14</v>
-      </c>
-      <c r="D12" s="1">
-        <v>1</v>
-      </c>
-      <c r="E12" s="1">
-        <v>15</v>
-      </c>
-      <c r="F12" s="1">
-        <v>1</v>
-      </c>
-      <c r="G12" s="1">
-        <v>14</v>
+      <c r="C12" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>127</v>
       </c>
       <c r="H12" s="1">
-        <v>2</v>
-      </c>
-      <c r="M12" s="1">
-        <v>3</v>
-      </c>
-      <c r="N12" s="16">
+        <v>3</v>
+      </c>
+      <c r="I12" s="16">
         <f t="shared" si="2"/>
         <v>4.4499999999999984</v>
       </c>
-      <c r="O12" s="7">
-        <f>ROUND(constants!B$3 * $M12 * $N12,0)</f>
+      <c r="J12" s="7">
+        <f>ROUND(constants!B$3 * $H12 * $I12,0)</f>
         <v>668</v>
       </c>
-      <c r="P12" s="7">
-        <f>ROUND(constants!C$3 * $M12 * $N12,0)</f>
+      <c r="K12" s="7">
+        <f>ROUND(constants!C$3 * $H12 * $I12,0)</f>
         <v>267</v>
       </c>
-      <c r="Q12" s="7">
-        <f>ROUND(constants!D$3 /4 * $N12,0)</f>
+      <c r="L12" s="7">
+        <f>ROUND(constants!D$3 /4 * $I12,0)</f>
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
+      <c r="I13" s="8"/>
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>
       <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="7"/>
-      <c r="P13" s="7"/>
-      <c r="Q13" s="7"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="9">
         <v>2</v>
       </c>
       <c r="B14" s="9">
         <v>1</v>
       </c>
-      <c r="C14" s="1">
-        <v>14</v>
-      </c>
-      <c r="D14" s="1">
+      <c r="C14" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H14" s="1">
+        <v>1</v>
+      </c>
+      <c r="I14" s="16">
         <v>4</v>
       </c>
-      <c r="M14" s="1">
-        <v>1</v>
-      </c>
-      <c r="N14" s="16">
-        <v>4</v>
-      </c>
-      <c r="O14" s="7">
-        <f>ROUND(constants!B$4 * $M14 * $N14,0)</f>
+      <c r="J14" s="7">
+        <f>ROUND(constants!B$4 * $H14 * $I14,0)</f>
         <v>212</v>
       </c>
-      <c r="P14" s="7">
-        <f>ROUND(constants!C$4 * $M14 * $N14,0)</f>
+      <c r="K14" s="7">
+        <f>ROUND(constants!C$4 * $H14 * $I14,0)</f>
         <v>88</v>
       </c>
-      <c r="Q14" s="7">
-        <f>ROUND(constants!D$3 /4 * $N14,0)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="L14" s="7">
+        <f>ROUND(constants!D$4 /4 * $I14,0)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="9">
         <f>A14</f>
         <v>2</v>
@@ -9011,33 +8901,33 @@
         <f>B14+1</f>
         <v>2</v>
       </c>
-      <c r="C15" s="1">
-        <v>15</v>
-      </c>
-      <c r="D15" s="1">
-        <v>4</v>
-      </c>
-      <c r="M15" s="1">
-        <v>1</v>
-      </c>
-      <c r="N15" s="16">
-        <f>N14+0.05</f>
+      <c r="C15" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H15" s="1">
+        <v>2</v>
+      </c>
+      <c r="I15" s="16">
+        <f>I14+0.05</f>
         <v>4.05</v>
       </c>
-      <c r="O15" s="7">
-        <f>ROUND(constants!B$4 * $M15 * $N15,0)</f>
-        <v>215</v>
-      </c>
-      <c r="P15" s="7">
-        <f>ROUND(constants!C$4 * $M15 * $N15,0)</f>
-        <v>89</v>
-      </c>
-      <c r="Q15" s="7">
-        <f>ROUND(constants!D$3 /4 * $N15,0)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="J15" s="7">
+        <f>ROUND(constants!B$4 * $H15 * $I15,0)</f>
+        <v>429</v>
+      </c>
+      <c r="K15" s="7">
+        <f>ROUND(constants!C$4 * $H15 * $I15,0)</f>
+        <v>178</v>
+      </c>
+      <c r="L15" s="7">
+        <f>ROUND(constants!D$4 /4 * $I15,0)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="9">
         <f t="shared" ref="A16:A27" si="3">A15</f>
         <v>2</v>
@@ -9046,39 +8936,30 @@
         <f>B15+1</f>
         <v>3</v>
       </c>
-      <c r="C16" s="1">
-        <v>12</v>
-      </c>
-      <c r="D16" s="1">
-        <v>5</v>
-      </c>
-      <c r="E16" s="1">
-        <v>16</v>
-      </c>
-      <c r="F16" s="1">
-        <v>4</v>
-      </c>
-      <c r="M16" s="1">
-        <v>2</v>
-      </c>
-      <c r="N16" s="16">
-        <f t="shared" ref="N16:N27" si="4">N15+0.05</f>
+      <c r="C16" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="H16" s="23">
+        <v>1</v>
+      </c>
+      <c r="I16" s="16">
+        <f t="shared" ref="I16:I27" si="4">I15+0.05</f>
         <v>4.0999999999999996</v>
       </c>
-      <c r="O16" s="7">
-        <f>ROUND(constants!B$4 * $M16 * $N16,0)</f>
-        <v>435</v>
-      </c>
-      <c r="P16" s="7">
-        <f>ROUND(constants!C$4 * $M16 * $N16,0)</f>
-        <v>180</v>
-      </c>
-      <c r="Q16" s="7">
-        <f>ROUND(constants!D$3 /4 * $N16,0)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="J16" s="7">
+        <f>ROUND(constants!B$4 * $H16 * $I16,0)</f>
+        <v>217</v>
+      </c>
+      <c r="K16" s="7">
+        <f>ROUND(constants!C$4 * $H16 * $I16,0)</f>
+        <v>90</v>
+      </c>
+      <c r="L16" s="7">
+        <f>ROUND(constants!D$4 /4 * $I16,0)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="9">
         <f t="shared" si="3"/>
         <v>2</v>
@@ -9087,33 +8968,33 @@
         <f t="shared" ref="B17:B22" si="5">B16+1</f>
         <v>4</v>
       </c>
-      <c r="C17" s="1">
-        <v>17</v>
-      </c>
-      <c r="D17" s="1">
-        <v>4</v>
-      </c>
-      <c r="M17" s="1">
-        <v>1</v>
-      </c>
-      <c r="N17" s="16">
+      <c r="C17" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="H17" s="1">
+        <v>2</v>
+      </c>
+      <c r="I17" s="16">
         <f t="shared" si="4"/>
         <v>4.1499999999999995</v>
       </c>
-      <c r="O17" s="7">
-        <f>ROUND(constants!B$4 * $M17 * $N17,0)</f>
-        <v>220</v>
-      </c>
-      <c r="P17" s="7">
-        <f>ROUND(constants!C$4 * $M17 * $N17,0)</f>
-        <v>91</v>
-      </c>
-      <c r="Q17" s="7">
-        <f>ROUND(constants!D$3 /4 * $N17,0)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="J17" s="7">
+        <f>ROUND(constants!B$4 * $H17 * $I17,0)</f>
+        <v>440</v>
+      </c>
+      <c r="K17" s="7">
+        <f>ROUND(constants!C$4 * $H17 * $I17,0)</f>
+        <v>183</v>
+      </c>
+      <c r="L17" s="7">
+        <f>ROUND(constants!D$4 /4 * $I17,0)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="9">
         <f t="shared" si="3"/>
         <v>2</v>
@@ -9122,39 +9003,36 @@
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
-      <c r="C18" s="1">
-        <v>12</v>
-      </c>
-      <c r="D18" s="1">
-        <v>4</v>
-      </c>
-      <c r="E18" s="1">
-        <v>12</v>
-      </c>
-      <c r="F18" s="1">
-        <v>5</v>
-      </c>
-      <c r="M18" s="1">
-        <v>2</v>
-      </c>
-      <c r="N18" s="16">
+      <c r="C18" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H18" s="1">
+        <v>3</v>
+      </c>
+      <c r="I18" s="16">
         <f t="shared" si="4"/>
         <v>4.1999999999999993</v>
       </c>
-      <c r="O18" s="7">
-        <f>ROUND(constants!B$4 * $M18 * $N18,0)</f>
-        <v>445</v>
-      </c>
-      <c r="P18" s="7">
-        <f>ROUND(constants!C$4 * $M18 * $N18,0)</f>
-        <v>185</v>
-      </c>
-      <c r="Q18" s="7">
-        <f>ROUND(constants!D$3 /4 * $N18,0)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="J18" s="7">
+        <f>ROUND(constants!B$4 * $H18 * $I18,0)</f>
+        <v>668</v>
+      </c>
+      <c r="K18" s="7">
+        <f>ROUND(constants!C$4 * $H18 * $I18,0)</f>
+        <v>277</v>
+      </c>
+      <c r="L18" s="7">
+        <f>ROUND(constants!D$4 /4 * $I18,0)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="9">
         <f t="shared" si="3"/>
         <v>2</v>
@@ -9163,39 +9041,33 @@
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
-      <c r="C19" s="1">
-        <v>13</v>
-      </c>
-      <c r="D19" s="1">
-        <v>4</v>
-      </c>
-      <c r="E19" s="1">
-        <v>15</v>
-      </c>
-      <c r="F19" s="1">
-        <v>4</v>
-      </c>
-      <c r="M19" s="1">
-        <v>2</v>
-      </c>
-      <c r="N19" s="16">
+      <c r="C19" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="H19" s="1">
+        <v>2</v>
+      </c>
+      <c r="I19" s="16">
         <f t="shared" si="4"/>
         <v>4.2499999999999991</v>
       </c>
-      <c r="O19" s="7">
-        <f>ROUND(constants!B$4 * $M19 * $N19,0)</f>
+      <c r="J19" s="7">
+        <f>ROUND(constants!B$4 * $H19 * $I19,0)</f>
         <v>451</v>
       </c>
-      <c r="P19" s="7">
-        <f>ROUND(constants!C$4 * $M19 * $N19,0)</f>
+      <c r="K19" s="7">
+        <f>ROUND(constants!C$4 * $H19 * $I19,0)</f>
         <v>187</v>
       </c>
-      <c r="Q19" s="7">
-        <f>ROUND(constants!D$3 /4 * $N19,0)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="L19" s="7">
+        <f>ROUND(constants!D$4 /4 * $I19,0)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="9">
         <f t="shared" si="3"/>
         <v>2</v>
@@ -9204,33 +9076,33 @@
         <f t="shared" si="5"/>
         <v>7</v>
       </c>
-      <c r="C20" s="1">
-        <v>14</v>
-      </c>
-      <c r="D20" s="1">
-        <v>5</v>
-      </c>
-      <c r="M20" s="1">
-        <v>1</v>
-      </c>
-      <c r="N20" s="16">
+      <c r="C20" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="H20" s="1">
+        <v>2</v>
+      </c>
+      <c r="I20" s="16">
         <f t="shared" si="4"/>
         <v>4.2999999999999989</v>
       </c>
-      <c r="O20" s="7">
-        <f>ROUND(constants!B$4 * $M20 * $N20,0)</f>
-        <v>228</v>
-      </c>
-      <c r="P20" s="7">
-        <f>ROUND(constants!C$4 * $M20 * $N20,0)</f>
-        <v>95</v>
-      </c>
-      <c r="Q20" s="7">
-        <f>ROUND(constants!D$3 /4 * $N20,0)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="J20" s="7">
+        <f>ROUND(constants!B$4 * $H20 * $I20,0)</f>
+        <v>456</v>
+      </c>
+      <c r="K20" s="7">
+        <f>ROUND(constants!C$4 * $H20 * $I20,0)</f>
+        <v>189</v>
+      </c>
+      <c r="L20" s="7">
+        <f>ROUND(constants!D$4 /4 * $I20,0)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="9">
         <f t="shared" si="3"/>
         <v>2</v>
@@ -9239,45 +9111,30 @@
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="C21" s="1">
-        <v>14</v>
-      </c>
-      <c r="D21" s="1">
-        <v>4</v>
-      </c>
-      <c r="E21" s="1">
-        <v>14</v>
-      </c>
-      <c r="F21" s="1">
-        <v>5</v>
-      </c>
-      <c r="G21" s="1">
-        <v>17</v>
-      </c>
-      <c r="H21" s="1">
-        <v>4</v>
-      </c>
-      <c r="M21" s="1">
-        <v>3</v>
-      </c>
-      <c r="N21" s="16">
+      <c r="C21" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H21" s="23">
+        <v>1</v>
+      </c>
+      <c r="I21" s="16">
         <f t="shared" si="4"/>
         <v>4.3499999999999988</v>
       </c>
-      <c r="O21" s="7">
-        <f>ROUND(constants!B$4 * $M21 * $N21,0)</f>
-        <v>692</v>
-      </c>
-      <c r="P21" s="7">
-        <f>ROUND(constants!C$4 * $M21 * $N21,0)</f>
-        <v>287</v>
-      </c>
-      <c r="Q21" s="7">
-        <f>ROUND(constants!D$3 /4 * $N21,0)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="J21" s="7">
+        <f>ROUND(constants!B$4 * $H21 * $I21,0)</f>
+        <v>231</v>
+      </c>
+      <c r="K21" s="7">
+        <f>ROUND(constants!C$4 * $H21 * $I21,0)</f>
+        <v>96</v>
+      </c>
+      <c r="L21" s="7">
+        <f>ROUND(constants!D$4 /4 * $I21,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="9">
         <f t="shared" si="3"/>
         <v>2</v>
@@ -9286,39 +9143,33 @@
         <f t="shared" si="5"/>
         <v>9</v>
       </c>
-      <c r="C22" s="1">
-        <v>13</v>
-      </c>
-      <c r="D22" s="1">
-        <v>4</v>
-      </c>
-      <c r="E22" s="1">
-        <v>15</v>
-      </c>
-      <c r="F22" s="1">
-        <v>4</v>
-      </c>
-      <c r="M22" s="1">
-        <v>2</v>
-      </c>
-      <c r="N22" s="16">
+      <c r="C22" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="H22" s="1">
+        <v>2</v>
+      </c>
+      <c r="I22" s="16">
         <f t="shared" si="4"/>
         <v>4.3999999999999986</v>
       </c>
-      <c r="O22" s="7">
-        <f>ROUND(constants!B$4 * $M22 * $N22,0)</f>
+      <c r="J22" s="7">
+        <f>ROUND(constants!B$4 * $H22 * $I22,0)</f>
         <v>466</v>
       </c>
-      <c r="P22" s="7">
-        <f>ROUND(constants!C$4 * $M22 * $N22,0)</f>
+      <c r="K22" s="7">
+        <f>ROUND(constants!C$4 * $H22 * $I22,0)</f>
         <v>194</v>
       </c>
-      <c r="Q22" s="7">
-        <f>ROUND(constants!D$3 /4 * $N22,0)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="L22" s="7">
+        <f>ROUND(constants!D$4 /4 * $I22,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="9">
         <f t="shared" si="3"/>
         <v>2</v>
@@ -9327,39 +9178,33 @@
         <f>B22+1</f>
         <v>10</v>
       </c>
-      <c r="C23" s="1">
-        <v>15</v>
-      </c>
-      <c r="D23" s="1">
-        <v>4</v>
-      </c>
-      <c r="E23" s="1">
-        <v>13</v>
-      </c>
-      <c r="F23" s="1">
-        <v>5</v>
-      </c>
-      <c r="M23" s="1">
-        <v>2</v>
-      </c>
-      <c r="N23" s="16">
+      <c r="C23" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H23" s="1">
+        <v>2</v>
+      </c>
+      <c r="I23" s="16">
         <f t="shared" si="4"/>
         <v>4.4499999999999984</v>
       </c>
-      <c r="O23" s="7">
-        <f>ROUND(constants!B$4 * $M23 * $N23,0)</f>
+      <c r="J23" s="7">
+        <f>ROUND(constants!B$4 * $H23 * $I23,0)</f>
         <v>472</v>
       </c>
-      <c r="P23" s="7">
-        <f>ROUND(constants!C$4 * $M23 * $N23,0)</f>
+      <c r="K23" s="7">
+        <f>ROUND(constants!C$4 * $H23 * $I23,0)</f>
         <v>196</v>
       </c>
-      <c r="Q23" s="7">
-        <f>ROUND(constants!D$3 /4 * $N23,0)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="L23" s="7">
+        <f>ROUND(constants!D$4 /4 * $I23,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="9">
         <f t="shared" si="3"/>
         <v>2</v>
@@ -9368,39 +9213,36 @@
         <f t="shared" ref="B24:B27" si="6">B23+1</f>
         <v>11</v>
       </c>
-      <c r="C24" s="1">
-        <v>12</v>
-      </c>
-      <c r="D24" s="1">
-        <v>5</v>
-      </c>
-      <c r="E24" s="1">
-        <v>16</v>
-      </c>
-      <c r="F24" s="1">
-        <v>4</v>
-      </c>
-      <c r="M24" s="1">
-        <v>2</v>
-      </c>
-      <c r="N24" s="16">
+      <c r="C24" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H24" s="1">
+        <v>3</v>
+      </c>
+      <c r="I24" s="16">
         <f t="shared" si="4"/>
         <v>4.4999999999999982</v>
       </c>
-      <c r="O24" s="7">
-        <f>ROUND(constants!B$4 * $M24 * $N24,0)</f>
-        <v>477</v>
-      </c>
-      <c r="P24" s="7">
-        <f>ROUND(constants!C$4 * $M24 * $N24,0)</f>
-        <v>198</v>
-      </c>
-      <c r="Q24" s="7">
-        <f>ROUND(constants!D$3 /4 * $N24,0)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="J24" s="7">
+        <f>ROUND(constants!B$4 * $H24 * $I24,0)</f>
+        <v>716</v>
+      </c>
+      <c r="K24" s="7">
+        <f>ROUND(constants!C$4 * $H24 * $I24,0)</f>
+        <v>297</v>
+      </c>
+      <c r="L24" s="7">
+        <f>ROUND(constants!D$4 /4 * $I24,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="9">
         <f t="shared" si="3"/>
         <v>2</v>
@@ -9409,45 +9251,36 @@
         <f t="shared" si="6"/>
         <v>12</v>
       </c>
-      <c r="C25" s="1">
-        <v>13</v>
-      </c>
-      <c r="D25" s="1">
-        <v>4</v>
-      </c>
-      <c r="E25" s="1">
-        <v>13</v>
-      </c>
-      <c r="F25" s="1">
-        <v>5</v>
-      </c>
-      <c r="G25" s="1">
-        <v>17</v>
+      <c r="C25" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="H25" s="1">
-        <v>4</v>
-      </c>
-      <c r="M25" s="1">
-        <v>3</v>
-      </c>
-      <c r="N25" s="16">
+        <v>3</v>
+      </c>
+      <c r="I25" s="16">
         <f t="shared" si="4"/>
         <v>4.549999999999998</v>
       </c>
-      <c r="O25" s="7">
-        <f>ROUND(constants!B$4 * $M25 * $N25,0)</f>
+      <c r="J25" s="7">
+        <f>ROUND(constants!B$4 * $H25 * $I25,0)</f>
         <v>723</v>
       </c>
-      <c r="P25" s="7">
-        <f>ROUND(constants!C$4 * $M25 * $N25,0)</f>
+      <c r="K25" s="7">
+        <f>ROUND(constants!C$4 * $H25 * $I25,0)</f>
         <v>300</v>
       </c>
-      <c r="Q25" s="7">
-        <f>ROUND(constants!D$3 /4 * $N25,0)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="L25" s="7">
+        <f>ROUND(constants!D$4 /4 * $I25,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="9">
         <f t="shared" si="3"/>
         <v>2</v>
@@ -9456,40 +9289,33 @@
         <f t="shared" si="6"/>
         <v>13</v>
       </c>
-      <c r="C26" s="1">
-        <v>16</v>
-      </c>
-      <c r="D26" s="1">
-        <v>4</v>
-      </c>
-      <c r="E26" s="1">
-        <v>14</v>
-      </c>
-      <c r="F26" s="1">
-        <v>5</v>
-      </c>
-      <c r="I26" s="7"/>
-      <c r="M26" s="1">
-        <v>2</v>
-      </c>
-      <c r="N26" s="16">
+      <c r="C26" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H26" s="1">
+        <v>2</v>
+      </c>
+      <c r="I26" s="16">
         <f t="shared" si="4"/>
         <v>4.5999999999999979</v>
       </c>
-      <c r="O26" s="7">
-        <f>ROUND(constants!B$4 * $M26 * $N26,0)</f>
+      <c r="J26" s="7">
+        <f>ROUND(constants!B$4 * $H26 * $I26,0)</f>
         <v>488</v>
       </c>
-      <c r="P26" s="7">
-        <f>ROUND(constants!C$4 * $M26 * $N26,0)</f>
+      <c r="K26" s="7">
+        <f>ROUND(constants!C$4 * $H26 * $I26,0)</f>
         <v>202</v>
       </c>
-      <c r="Q26" s="7">
-        <f>ROUND(constants!D$3 /4 * $N26,0)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="L26" s="7">
+        <f>ROUND(constants!D$4 /4 * $I26,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="9">
         <f t="shared" si="3"/>
         <v>2</v>
@@ -9498,81 +9324,69 @@
         <f t="shared" si="6"/>
         <v>14</v>
       </c>
-      <c r="C27" s="1">
-        <v>14</v>
-      </c>
-      <c r="D27" s="1">
-        <v>4</v>
-      </c>
-      <c r="E27" s="1">
-        <v>13</v>
-      </c>
-      <c r="F27" s="1">
-        <v>5</v>
-      </c>
-      <c r="G27" s="1">
-        <v>16</v>
+      <c r="C27" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>127</v>
       </c>
       <c r="H27" s="1">
-        <v>5</v>
-      </c>
-      <c r="M27" s="1">
-        <v>3</v>
-      </c>
-      <c r="N27" s="16">
+        <v>3</v>
+      </c>
+      <c r="I27" s="16">
         <f t="shared" si="4"/>
         <v>4.6499999999999977</v>
       </c>
-      <c r="O27" s="7">
-        <f>ROUND(constants!B$4 * $M27 * $N27,0)</f>
+      <c r="J27" s="7">
+        <f>ROUND(constants!B$4 * $H27 * $I27,0)</f>
         <v>739</v>
       </c>
-      <c r="P27" s="7">
-        <f>ROUND(constants!C$4 * $M27 * $N27,0)</f>
+      <c r="K27" s="7">
+        <f>ROUND(constants!C$4 * $H27 * $I27,0)</f>
         <v>307</v>
       </c>
-      <c r="Q27" s="7">
-        <f>ROUND(constants!D$3 /4 * $N27,0)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="N28" s="15"/>
-      <c r="P28" s="7"/>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="L27" s="7">
+        <f>ROUND(constants!D$4 /4 * $I27,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I28" s="15"/>
+      <c r="K28" s="7"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="9">
         <v>3</v>
       </c>
       <c r="B29" s="9">
         <v>1</v>
       </c>
-      <c r="C29" s="1">
-        <v>16</v>
-      </c>
-      <c r="D29" s="1">
+      <c r="C29" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H29" s="1">
+        <v>1</v>
+      </c>
+      <c r="I29" s="16">
+        <v>4</v>
+      </c>
+      <c r="J29" s="7">
+        <f>ROUND(constants!B$5 * $H29 * $I29,0)</f>
+        <v>224</v>
+      </c>
+      <c r="K29" s="7">
+        <f>ROUND(constants!C$5 * $H29 * $I29,0)</f>
+        <v>96</v>
+      </c>
+      <c r="L29" s="7">
+        <f>ROUND(constants!D$5 /4 * $I29,0)</f>
         <v>7</v>
       </c>
-      <c r="M29" s="1">
-        <v>1</v>
-      </c>
-      <c r="N29" s="16">
-        <v>4</v>
-      </c>
-      <c r="O29" s="7">
-        <f>ROUND(constants!B$5 * $M29 * $N29,0)</f>
-        <v>224</v>
-      </c>
-      <c r="P29" s="7">
-        <f>ROUND(constants!C$5 * $M29 * $N29,0)</f>
-        <v>96</v>
-      </c>
-      <c r="Q29" s="7">
-        <f>ROUND(constants!D$3 /4 * $N29,0)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="9">
         <f>A29</f>
         <v>3</v>
@@ -9581,39 +9395,33 @@
         <f>B29+1</f>
         <v>2</v>
       </c>
-      <c r="C30" s="1">
-        <v>13</v>
-      </c>
-      <c r="D30" s="1">
+      <c r="C30" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H30" s="1">
+        <v>2</v>
+      </c>
+      <c r="I30" s="16">
+        <f>I29+0.05</f>
+        <v>4.05</v>
+      </c>
+      <c r="J30" s="7">
+        <f>ROUND(constants!B$5 * $H30 * $I30,0)</f>
+        <v>454</v>
+      </c>
+      <c r="K30" s="7">
+        <f>ROUND(constants!C$5 * $H30 * $I30,0)</f>
+        <v>194</v>
+      </c>
+      <c r="L30" s="7">
+        <f>ROUND(constants!D$5 /4 * $I30,0)</f>
         <v>7</v>
       </c>
-      <c r="E30" s="1">
-        <v>17</v>
-      </c>
-      <c r="F30" s="1">
-        <v>7</v>
-      </c>
-      <c r="M30" s="1">
-        <v>2</v>
-      </c>
-      <c r="N30" s="16">
-        <f>N29+0.05</f>
-        <v>4.05</v>
-      </c>
-      <c r="O30" s="7">
-        <f>ROUND(constants!B$5 * $M30 * $N30,0)</f>
-        <v>454</v>
-      </c>
-      <c r="P30" s="7">
-        <f>ROUND(constants!C$5 * $M30 * $N30,0)</f>
-        <v>194</v>
-      </c>
-      <c r="Q30" s="7">
-        <f>ROUND(constants!D$3 /4 * $N30,0)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="9">
         <f t="shared" ref="A31:A45" si="7">A30</f>
         <v>3</v>
@@ -9622,35 +9430,34 @@
         <f>B30+1</f>
         <v>3</v>
       </c>
-      <c r="C31" s="1">
-        <v>18</v>
-      </c>
-      <c r="D31" s="1">
+      <c r="C31" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G31" s="7"/>
+      <c r="H31" s="1">
+        <v>2</v>
+      </c>
+      <c r="I31" s="16">
+        <f t="shared" ref="I31:I45" si="8">I30+0.05</f>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="J31" s="7">
+        <f>ROUND(constants!B$5 * $H31 * $I31,0)</f>
+        <v>459</v>
+      </c>
+      <c r="K31" s="7">
+        <f>ROUND(constants!C$5 * $H31 * $I31,0)</f>
+        <v>197</v>
+      </c>
+      <c r="L31" s="7">
+        <f>ROUND(constants!D$5 /4 * $I31,0)</f>
         <v>7</v>
       </c>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-      <c r="M31" s="1">
-        <v>1</v>
-      </c>
-      <c r="N31" s="16">
-        <f t="shared" ref="N31:N45" si="8">N30+0.05</f>
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="O31" s="7">
-        <f>ROUND(constants!B$5 * $M31 * $N31,0)</f>
-        <v>230</v>
-      </c>
-      <c r="P31" s="7">
-        <f>ROUND(constants!C$5 * $M31 * $N31,0)</f>
-        <v>98</v>
-      </c>
-      <c r="Q31" s="7">
-        <f>ROUND(constants!D$3 /4 * $N31,0)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="9">
         <f t="shared" si="7"/>
         <v>3</v>
@@ -9659,45 +9466,30 @@
         <f t="shared" ref="B32:B37" si="9">B31+1</f>
         <v>4</v>
       </c>
-      <c r="C32" s="1">
-        <v>15</v>
-      </c>
-      <c r="D32" s="1">
-        <v>7</v>
-      </c>
-      <c r="E32" s="1">
-        <v>12</v>
-      </c>
-      <c r="F32" s="1">
-        <v>8</v>
-      </c>
-      <c r="G32" s="1">
-        <v>19</v>
-      </c>
-      <c r="H32" s="1">
-        <v>7</v>
-      </c>
-      <c r="M32" s="1">
-        <v>3</v>
-      </c>
-      <c r="N32" s="16">
+      <c r="C32" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="H32" s="23">
+        <v>1</v>
+      </c>
+      <c r="I32" s="16">
         <f t="shared" si="8"/>
         <v>4.1499999999999995</v>
       </c>
-      <c r="O32" s="7">
-        <f>ROUND(constants!B$5 * $M32 * $N32,0)</f>
-        <v>697</v>
-      </c>
-      <c r="P32" s="7">
-        <f>ROUND(constants!C$5 * $M32 * $N32,0)</f>
-        <v>299</v>
-      </c>
-      <c r="Q32" s="7">
-        <f>ROUND(constants!D$3 /4 * $N32,0)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="J32" s="7">
+        <f>ROUND(constants!B$5 * $H32 * $I32,0)</f>
+        <v>232</v>
+      </c>
+      <c r="K32" s="7">
+        <f>ROUND(constants!C$5 * $H32 * $I32,0)</f>
+        <v>100</v>
+      </c>
+      <c r="L32" s="7">
+        <f>ROUND(constants!D$5 /4 * $I32,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="9">
         <f t="shared" si="7"/>
         <v>3</v>
@@ -9706,39 +9498,33 @@
         <f t="shared" si="9"/>
         <v>5</v>
       </c>
-      <c r="C33" s="1">
-        <v>14</v>
-      </c>
-      <c r="D33" s="1">
-        <v>7</v>
-      </c>
-      <c r="E33" s="1">
-        <v>16</v>
-      </c>
-      <c r="F33" s="1">
-        <v>7</v>
-      </c>
-      <c r="M33" s="1">
-        <v>2</v>
-      </c>
-      <c r="N33" s="16">
+      <c r="C33" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="H33" s="1">
+        <v>2</v>
+      </c>
+      <c r="I33" s="16">
         <f t="shared" si="8"/>
         <v>4.1999999999999993</v>
       </c>
-      <c r="O33" s="7">
-        <f>ROUND(constants!B$5 * $M33 * $N33,0)</f>
+      <c r="J33" s="7">
+        <f>ROUND(constants!B$5 * $H33 * $I33,0)</f>
         <v>470</v>
       </c>
-      <c r="P33" s="7">
-        <f>ROUND(constants!C$5 * $M33 * $N33,0)</f>
+      <c r="K33" s="7">
+        <f>ROUND(constants!C$5 * $H33 * $I33,0)</f>
         <v>202</v>
       </c>
-      <c r="Q33" s="7">
-        <f>ROUND(constants!D$3 /4 * $N33,0)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="L33" s="7">
+        <f>ROUND(constants!D$5 /4 * $I33,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="9">
         <f t="shared" si="7"/>
         <v>3</v>
@@ -9747,35 +9533,31 @@
         <f t="shared" si="9"/>
         <v>6</v>
       </c>
-      <c r="C34" s="1">
-        <v>15</v>
-      </c>
-      <c r="D34" s="1">
-        <v>8</v>
+      <c r="C34" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="G34" s="7"/>
-      <c r="H34" s="7"/>
-      <c r="M34" s="1">
-        <v>1</v>
-      </c>
-      <c r="N34" s="16">
+      <c r="H34" s="1">
+        <v>1</v>
+      </c>
+      <c r="I34" s="16">
         <f t="shared" si="8"/>
         <v>4.2499999999999991</v>
       </c>
-      <c r="O34" s="7">
-        <f>ROUND(constants!B$5 * $M34 * $N34,0)</f>
+      <c r="J34" s="7">
+        <f>ROUND(constants!B$5 * $H34 * $I34,0)</f>
         <v>238</v>
       </c>
-      <c r="P34" s="7">
-        <f>ROUND(constants!C$5 * $M34 * $N34,0)</f>
+      <c r="K34" s="7">
+        <f>ROUND(constants!C$5 * $H34 * $I34,0)</f>
         <v>102</v>
       </c>
-      <c r="Q34" s="7">
-        <f>ROUND(constants!D$3 /4 * $N34,0)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="L34" s="7">
+        <f>ROUND(constants!D$5 /4 * $I34,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="9">
         <f t="shared" si="7"/>
         <v>3</v>
@@ -9784,39 +9566,33 @@
         <f t="shared" si="9"/>
         <v>7</v>
       </c>
-      <c r="C35" s="1">
-        <v>16</v>
-      </c>
-      <c r="D35" s="1">
-        <v>7</v>
-      </c>
-      <c r="E35" s="1">
-        <v>16</v>
-      </c>
-      <c r="F35" s="1">
-        <v>8</v>
-      </c>
-      <c r="M35" s="1">
-        <v>2</v>
-      </c>
-      <c r="N35" s="16">
+      <c r="C35" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="H35" s="1">
+        <v>2</v>
+      </c>
+      <c r="I35" s="16">
         <f t="shared" si="8"/>
         <v>4.2999999999999989</v>
       </c>
-      <c r="O35" s="7">
-        <f>ROUND(constants!B$5 * $M35 * $N35,0)</f>
+      <c r="J35" s="7">
+        <f>ROUND(constants!B$5 * $H35 * $I35,0)</f>
         <v>482</v>
       </c>
-      <c r="P35" s="7">
-        <f>ROUND(constants!C$5 * $M35 * $N35,0)</f>
+      <c r="K35" s="7">
+        <f>ROUND(constants!C$5 * $H35 * $I35,0)</f>
         <v>206</v>
       </c>
-      <c r="Q35" s="7">
-        <f>ROUND(constants!D$3 /4 * $N35,0)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="L35" s="7">
+        <f>ROUND(constants!D$5 /4 * $I35,0)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="9">
         <f t="shared" si="7"/>
         <v>3</v>
@@ -9825,39 +9601,33 @@
         <f t="shared" si="9"/>
         <v>8</v>
       </c>
-      <c r="C36" s="1">
-        <v>13</v>
-      </c>
-      <c r="D36" s="1">
-        <v>8</v>
-      </c>
-      <c r="E36" s="1">
-        <v>19</v>
-      </c>
-      <c r="F36" s="1">
-        <v>7</v>
-      </c>
-      <c r="M36" s="1">
-        <v>2</v>
-      </c>
-      <c r="N36" s="16">
+      <c r="C36" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="H36" s="1">
+        <v>2</v>
+      </c>
+      <c r="I36" s="16">
         <f t="shared" si="8"/>
         <v>4.3499999999999988</v>
       </c>
-      <c r="O36" s="7">
-        <f>ROUND(constants!B$5 * $M36 * $N36,0)</f>
+      <c r="J36" s="7">
+        <f>ROUND(constants!B$5 * $H36 * $I36,0)</f>
         <v>487</v>
       </c>
-      <c r="P36" s="7">
-        <f>ROUND(constants!C$5 * $M36 * $N36,0)</f>
+      <c r="K36" s="7">
+        <f>ROUND(constants!C$5 * $H36 * $I36,0)</f>
         <v>209</v>
       </c>
-      <c r="Q36" s="7">
-        <f>ROUND(constants!D$3 /4 * $N36,0)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="L36" s="7">
+        <f>ROUND(constants!D$5 /4 * $I36,0)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="9">
         <f t="shared" si="7"/>
         <v>3</v>
@@ -9866,45 +9636,36 @@
         <f t="shared" si="9"/>
         <v>9</v>
       </c>
-      <c r="C37" s="1">
-        <v>13</v>
-      </c>
-      <c r="D37" s="1">
-        <v>7</v>
-      </c>
-      <c r="E37" s="1">
-        <v>16</v>
-      </c>
-      <c r="F37" s="1">
-        <v>7</v>
-      </c>
-      <c r="G37" s="1">
-        <v>14</v>
+      <c r="C37" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="H37" s="1">
-        <v>8</v>
-      </c>
-      <c r="M37" s="1">
-        <v>3</v>
-      </c>
-      <c r="N37" s="16">
+        <v>3</v>
+      </c>
+      <c r="I37" s="16">
         <f t="shared" si="8"/>
         <v>4.3999999999999986</v>
       </c>
-      <c r="O37" s="7">
-        <f>ROUND(constants!B$5 * $M37 * $N37,0)</f>
+      <c r="J37" s="7">
+        <f>ROUND(constants!B$5 * $H37 * $I37,0)</f>
         <v>739</v>
       </c>
-      <c r="P37" s="7">
-        <f>ROUND(constants!C$5 * $M37 * $N37,0)</f>
+      <c r="K37" s="7">
+        <f>ROUND(constants!C$5 * $H37 * $I37,0)</f>
         <v>317</v>
       </c>
-      <c r="Q37" s="7">
-        <f>ROUND(constants!D$3 /4 * $N37,0)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="L37" s="7">
+        <f>ROUND(constants!D$5 /4 * $I37,0)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="9">
         <f t="shared" si="7"/>
         <v>3</v>
@@ -9913,45 +9674,30 @@
         <f>B37+1</f>
         <v>10</v>
       </c>
-      <c r="C38" s="1">
-        <v>14</v>
-      </c>
-      <c r="D38" s="1">
-        <v>7</v>
-      </c>
-      <c r="E38" s="1">
-        <v>13</v>
-      </c>
-      <c r="F38" s="1">
-        <v>8</v>
-      </c>
-      <c r="G38" s="1">
-        <v>17</v>
-      </c>
-      <c r="H38" s="1">
-        <v>7</v>
-      </c>
-      <c r="M38" s="1">
-        <v>3</v>
-      </c>
-      <c r="N38" s="16">
+      <c r="C38" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H38" s="23">
+        <v>1</v>
+      </c>
+      <c r="I38" s="16">
         <f t="shared" si="8"/>
         <v>4.4499999999999984</v>
       </c>
-      <c r="O38" s="7">
-        <f>ROUND(constants!B$5 * $M38 * $N38,0)</f>
-        <v>748</v>
-      </c>
-      <c r="P38" s="7">
-        <f>ROUND(constants!C$5 * $M38 * $N38,0)</f>
-        <v>320</v>
-      </c>
-      <c r="Q38" s="7">
-        <f>ROUND(constants!D$3 /4 * $N38,0)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="J38" s="7">
+        <f>ROUND(constants!B$5 * $H38 * $I38,0)</f>
+        <v>249</v>
+      </c>
+      <c r="K38" s="7">
+        <f>ROUND(constants!C$5 * $H38 * $I38,0)</f>
+        <v>107</v>
+      </c>
+      <c r="L38" s="7">
+        <f>ROUND(constants!D$5 /4 * $I38,0)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="9">
         <f t="shared" si="7"/>
         <v>3</v>
@@ -9960,39 +9706,33 @@
         <f t="shared" ref="B39:B45" si="10">B38+1</f>
         <v>11</v>
       </c>
-      <c r="C39" s="1">
-        <v>14</v>
-      </c>
-      <c r="D39" s="1">
-        <v>8</v>
-      </c>
-      <c r="E39" s="1">
-        <v>18</v>
-      </c>
-      <c r="F39" s="1">
-        <v>7</v>
-      </c>
-      <c r="M39" s="1">
-        <v>2</v>
-      </c>
-      <c r="N39" s="16">
+      <c r="C39" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H39" s="1">
+        <v>2</v>
+      </c>
+      <c r="I39" s="16">
         <f t="shared" si="8"/>
         <v>4.4999999999999982</v>
       </c>
-      <c r="O39" s="7">
-        <f>ROUND(constants!B$5 * $M39 * $N39,0)</f>
+      <c r="J39" s="7">
+        <f>ROUND(constants!B$5 * $H39 * $I39,0)</f>
         <v>504</v>
       </c>
-      <c r="P39" s="7">
-        <f>ROUND(constants!C$5 * $M39 * $N39,0)</f>
+      <c r="K39" s="7">
+        <f>ROUND(constants!C$5 * $H39 * $I39,0)</f>
         <v>216</v>
       </c>
-      <c r="Q39" s="7">
-        <f>ROUND(constants!D$3 /4 * $N39,0)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="L39" s="7">
+        <f>ROUND(constants!D$5 /4 * $I39,0)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="9">
         <f t="shared" si="7"/>
         <v>3</v>
@@ -10001,33 +9741,30 @@
         <f t="shared" si="10"/>
         <v>12</v>
       </c>
-      <c r="C40" s="1">
-        <v>19</v>
-      </c>
-      <c r="D40" s="1">
-        <v>7</v>
-      </c>
-      <c r="M40" s="1">
-        <v>1</v>
-      </c>
-      <c r="N40" s="16">
+      <c r="C40" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="H40" s="1">
+        <v>1</v>
+      </c>
+      <c r="I40" s="16">
         <f t="shared" si="8"/>
         <v>4.549999999999998</v>
       </c>
-      <c r="O40" s="7">
-        <f>ROUND(constants!B$5 * $M40 * $N40,0)</f>
+      <c r="J40" s="7">
+        <f>ROUND(constants!B$5 * $H40 * $I40,0)</f>
         <v>255</v>
       </c>
-      <c r="P40" s="7">
-        <f>ROUND(constants!C$5 * $M40 * $N40,0)</f>
+      <c r="K40" s="7">
+        <f>ROUND(constants!C$5 * $H40 * $I40,0)</f>
         <v>109</v>
       </c>
-      <c r="Q40" s="7">
-        <f>ROUND(constants!D$3 /4 * $N40,0)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="L40" s="7">
+        <f>ROUND(constants!D$5 /4 * $I40,0)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="9">
         <f t="shared" si="7"/>
         <v>3</v>
@@ -10036,39 +9773,33 @@
         <f t="shared" si="10"/>
         <v>13</v>
       </c>
-      <c r="C41" s="1">
-        <v>16</v>
-      </c>
-      <c r="D41" s="1">
-        <v>7</v>
-      </c>
-      <c r="E41" s="1">
-        <v>14</v>
-      </c>
-      <c r="F41" s="1">
-        <v>8</v>
-      </c>
-      <c r="M41" s="1">
-        <v>2</v>
-      </c>
-      <c r="N41" s="16">
+      <c r="C41" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H41" s="1">
+        <v>2</v>
+      </c>
+      <c r="I41" s="16">
         <f t="shared" si="8"/>
         <v>4.5999999999999979</v>
       </c>
-      <c r="O41" s="7">
-        <f>ROUND(constants!B$5 * $M41 * $N41,0)</f>
+      <c r="J41" s="7">
+        <f>ROUND(constants!B$5 * $H41 * $I41,0)</f>
         <v>515</v>
       </c>
-      <c r="P41" s="7">
-        <f>ROUND(constants!C$5 * $M41 * $N41,0)</f>
+      <c r="K41" s="7">
+        <f>ROUND(constants!C$5 * $H41 * $I41,0)</f>
         <v>221</v>
       </c>
-      <c r="Q41" s="7">
-        <f>ROUND(constants!D$3 /4 * $N41,0)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="L41" s="7">
+        <f>ROUND(constants!D$5 /4 * $I41,0)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="9">
         <f t="shared" si="7"/>
         <v>3</v>
@@ -10077,45 +9808,36 @@
         <f t="shared" si="10"/>
         <v>14</v>
       </c>
-      <c r="C42" s="1">
-        <v>14</v>
-      </c>
-      <c r="D42" s="1">
-        <v>7</v>
-      </c>
-      <c r="E42" s="1">
-        <v>15</v>
-      </c>
-      <c r="F42" s="1">
-        <v>7</v>
-      </c>
-      <c r="G42" s="1">
-        <v>15</v>
+      <c r="C42" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>127</v>
       </c>
       <c r="H42" s="1">
-        <v>8</v>
-      </c>
-      <c r="M42" s="1">
-        <v>3</v>
-      </c>
-      <c r="N42" s="16">
+        <v>3</v>
+      </c>
+      <c r="I42" s="16">
         <f t="shared" si="8"/>
         <v>4.6499999999999977</v>
       </c>
-      <c r="O42" s="7">
-        <f>ROUND(constants!B$5 * $M42 * $N42,0)</f>
+      <c r="J42" s="7">
+        <f>ROUND(constants!B$5 * $H42 * $I42,0)</f>
         <v>781</v>
       </c>
-      <c r="P42" s="7">
-        <f>ROUND(constants!C$5 * $M42 * $N42,0)</f>
+      <c r="K42" s="7">
+        <f>ROUND(constants!C$5 * $H42 * $I42,0)</f>
         <v>335</v>
       </c>
-      <c r="Q42" s="7">
-        <f>ROUND(constants!D$3 /4 * $N42,0)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="L42" s="7">
+        <f>ROUND(constants!D$5 /4 * $I42,0)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="9">
         <f t="shared" si="7"/>
         <v>3</v>
@@ -10124,45 +9846,36 @@
         <f t="shared" si="10"/>
         <v>15</v>
       </c>
-      <c r="C43" s="1">
-        <v>13</v>
-      </c>
-      <c r="D43" s="1">
-        <v>7</v>
-      </c>
-      <c r="E43" s="1">
-        <v>14</v>
-      </c>
-      <c r="F43" s="1">
-        <v>8</v>
-      </c>
-      <c r="G43" s="1">
-        <v>18</v>
+      <c r="C43" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="H43" s="1">
-        <v>7</v>
-      </c>
-      <c r="M43" s="1">
-        <v>3</v>
-      </c>
-      <c r="N43" s="16">
+        <v>3</v>
+      </c>
+      <c r="I43" s="16">
         <f t="shared" si="8"/>
         <v>4.6999999999999975</v>
       </c>
-      <c r="O43" s="7">
-        <f>ROUND(constants!B$5 * $M43 * $N43,0)</f>
+      <c r="J43" s="7">
+        <f>ROUND(constants!B$5 * $H43 * $I43,0)</f>
         <v>790</v>
       </c>
-      <c r="P43" s="7">
-        <f>ROUND(constants!C$5 * $M43 * $N43,0)</f>
+      <c r="K43" s="7">
+        <f>ROUND(constants!C$5 * $H43 * $I43,0)</f>
         <v>338</v>
       </c>
-      <c r="Q43" s="7">
-        <f>ROUND(constants!D$3 /4 * $N43,0)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="L43" s="7">
+        <f>ROUND(constants!D$5 /4 * $I43,0)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" s="9">
         <f t="shared" si="7"/>
         <v>3</v>
@@ -10171,39 +9884,33 @@
         <f t="shared" si="10"/>
         <v>16</v>
       </c>
-      <c r="C44" s="1">
-        <v>17</v>
-      </c>
-      <c r="D44" s="1">
-        <v>7</v>
-      </c>
-      <c r="E44" s="1">
-        <v>19</v>
-      </c>
-      <c r="F44" s="1">
-        <v>7</v>
-      </c>
-      <c r="M44" s="1">
-        <v>2</v>
-      </c>
-      <c r="N44" s="16">
+      <c r="C44" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H44" s="1">
+        <v>2</v>
+      </c>
+      <c r="I44" s="16">
         <f t="shared" si="8"/>
         <v>4.7499999999999973</v>
       </c>
-      <c r="O44" s="7">
-        <f>ROUND(constants!B$5 * $M44 * $N44,0)</f>
+      <c r="J44" s="7">
+        <f>ROUND(constants!B$5 * $H44 * $I44,0)</f>
         <v>532</v>
       </c>
-      <c r="P44" s="7">
-        <f>ROUND(constants!C$5 * $M44 * $N44,0)</f>
+      <c r="K44" s="7">
+        <f>ROUND(constants!C$5 * $H44 * $I44,0)</f>
         <v>228</v>
       </c>
-      <c r="Q44" s="7">
-        <f>ROUND(constants!D$3 /4 * $N44,0)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="L44" s="7">
+        <f>ROUND(constants!D$5 /4 * $I44,0)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" s="9">
         <f t="shared" si="7"/>
         <v>3</v>
@@ -10212,42 +9919,33 @@
         <f t="shared" si="10"/>
         <v>17</v>
       </c>
-      <c r="C45" s="1">
-        <v>18</v>
-      </c>
-      <c r="D45" s="1">
-        <v>7</v>
-      </c>
-      <c r="E45" s="1">
-        <v>17</v>
-      </c>
-      <c r="F45" s="1">
-        <v>8</v>
-      </c>
-      <c r="G45" s="1">
-        <v>18</v>
+      <c r="C45" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>127</v>
       </c>
       <c r="H45" s="1">
-        <v>8</v>
-      </c>
-      <c r="M45" s="1">
-        <v>3</v>
-      </c>
-      <c r="N45" s="16">
+        <v>3</v>
+      </c>
+      <c r="I45" s="16">
         <f t="shared" si="8"/>
         <v>4.7999999999999972</v>
       </c>
-      <c r="O45" s="7">
-        <f>ROUND(constants!B$5 * $M45 * $N45,0)</f>
+      <c r="J45" s="7">
+        <f>ROUND(constants!B$5 * $H45 * $I45,0)</f>
         <v>806</v>
       </c>
-      <c r="P45" s="7">
-        <f>ROUND(constants!C$5 * $M45 * $N45,0)</f>
+      <c r="K45" s="7">
+        <f>ROUND(constants!C$5 * $H45 * $I45,0)</f>
         <v>346</v>
       </c>
-      <c r="Q45" s="7">
-        <f>ROUND(constants!D$3 /4 * $N45,0)</f>
-        <v>6</v>
+      <c r="L45" s="7">
+        <f>ROUND(constants!D$5 /4 * $I45,0)</f>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>